<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@a51df628d6007057972ae2e18b6811cf6ab369c1 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="269">
   <si>
     <t>Row</t>
   </si>
@@ -337,7 +337,16 @@
     <t>F1</t>
   </si>
   <si>
-    <t>~</t>
+    <t>Polyfuse 1.8A</t>
+  </si>
+  <si>
+    <t>C_Rect_L7.0mm_W3.5mm_P5.00mm</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Bel%20Fuse%20PDFs/0ZRP_Series.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bel-fuse-inc/0ZRP0090FF1E/9468255</t>
   </si>
   <si>
     <t>8</t>
@@ -574,6 +583,15 @@
     <t>2.2uH</t>
   </si>
   <si>
+    <t>L_Radial_D12.0mm_P5.00mm_Fastron_11P</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Wurth%20Electronics%20PDFs/7447471022.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/7447471022/2794428</t>
+  </si>
+  <si>
     <t>19</t>
   </si>
   <si>
@@ -844,7 +862,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>69 (0 SMD/ 57 THT)</t>
+    <t>69 (0 SMD/ 67 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -883,7 +901,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-26 20:36:06</t>
+    <t>2023-03-26 22:39:08</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
@@ -1683,7 +1701,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1697,13 +1715,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="F2" s="3">
         <v>34</v>
@@ -1711,41 +1729,41 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1753,13 +1771,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="F6" s="3">
         <v>69</v>
@@ -2031,7 +2049,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>61</v>
       </c>
@@ -2045,10 +2063,10 @@
         <v>64</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>22</v>
+        <v>65</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>12</v>
@@ -2056,11 +2074,11 @@
       <c r="H15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>22</v>
+      <c r="I15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>22</v>
@@ -2071,22 +2089,22 @@
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>12</v>
@@ -2095,10 +2113,10 @@
         <v>19</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>22</v>
@@ -2109,22 +2127,22 @@
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>43</v>
@@ -2133,10 +2151,10 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>22</v>
@@ -2150,19 +2168,19 @@
         <v>58</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>12</v>
@@ -2171,10 +2189,10 @@
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>22</v>
@@ -2185,22 +2203,22 @@
     </row>
     <row r="19" spans="1:12" ht="60" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>12</v>
@@ -2209,10 +2227,10 @@
         <v>19</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>22</v>
@@ -2226,19 +2244,19 @@
         <v>26</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>18</v>
@@ -2247,10 +2265,10 @@
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>22</v>
@@ -2261,22 +2279,22 @@
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>18</v>
@@ -2285,10 +2303,10 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>22</v>
@@ -2299,22 +2317,22 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>12</v>
@@ -2323,10 +2341,10 @@
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>22</v>
@@ -2337,22 +2355,22 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>12</v>
@@ -2361,10 +2379,10 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>22</v>
@@ -2375,22 +2393,22 @@
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>12</v>
@@ -2399,10 +2417,10 @@
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>22</v>
@@ -2413,22 +2431,22 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>12</v>
@@ -2437,10 +2455,10 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>22</v>
@@ -2449,24 +2467,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>22</v>
+        <v>146</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>147</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>12</v>
@@ -2474,11 +2492,11 @@
       <c r="H26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>22</v>
+      <c r="I26" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>22</v>
@@ -2489,22 +2507,22 @@
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>43</v>
@@ -2513,10 +2531,10 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>22</v>
@@ -2527,22 +2545,22 @@
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>12</v>
@@ -2551,10 +2569,10 @@
         <v>19</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>22</v>
@@ -2565,22 +2583,22 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
@@ -2589,10 +2607,10 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>22</v>
@@ -2603,22 +2621,22 @@
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>159</v>
-      </c>
       <c r="C30" s="11" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>12</v>
@@ -2627,10 +2645,10 @@
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>22</v>
@@ -2641,22 +2659,22 @@
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>12</v>
@@ -2665,10 +2683,10 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>22</v>
@@ -2679,22 +2697,22 @@
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>18</v>
@@ -2703,10 +2721,10 @@
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>22</v>
@@ -2717,22 +2735,22 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>12</v>
@@ -2741,10 +2759,10 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>22</v>
@@ -2755,22 +2773,22 @@
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="D34" s="11" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>12</v>
@@ -2779,10 +2797,10 @@
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>22</v>
@@ -2793,22 +2811,22 @@
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
@@ -2817,10 +2835,10 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>22</v>
@@ -2831,22 +2849,22 @@
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>50</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>12</v>
@@ -2855,10 +2873,10 @@
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>22</v>
@@ -2869,22 +2887,22 @@
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
@@ -2893,10 +2911,10 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>22</v>
@@ -2907,22 +2925,22 @@
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -2931,10 +2949,10 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>22</v>
@@ -2945,22 +2963,22 @@
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -2969,10 +2987,10 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>22</v>
@@ -2983,22 +3001,22 @@
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>200</v>
-      </c>
       <c r="D40" s="11" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3007,10 +3025,10 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>22</v>
@@ -3021,22 +3039,22 @@
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3045,10 +3063,10 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>22</v>
@@ -3059,22 +3077,22 @@
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>12</v>
@@ -3083,10 +3101,10 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>22</v>
@@ -3129,7 +3147,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3137,13 +3155,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3151,13 +3169,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3166,13 +3184,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G43)</f>
@@ -3181,23 +3199,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3217,16 +3235,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3361,15 +3379,18 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="30" customHeight="1">
       <c r="A16" s="19" t="s">
         <v>64</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>22</v>
+        <v>66</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>67</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -3382,16 +3403,16 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -3404,16 +3425,16 @@
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1">
       <c r="A18" s="19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E18" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -3426,16 +3447,16 @@
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E19" s="19">
         <f>BoardQty*1</f>
@@ -3448,16 +3469,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -3470,16 +3491,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3492,16 +3513,16 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E22" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3514,16 +3535,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E23" s="19">
         <f>BoardQty*1</f>
@@ -3536,16 +3557,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -3558,16 +3579,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -3580,16 +3601,16 @@
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -3600,15 +3621,18 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>22</v>
+        <v>147</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -3621,16 +3645,16 @@
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E28" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -3643,16 +3667,16 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -3665,16 +3689,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -3687,16 +3711,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -3709,16 +3733,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -3731,16 +3755,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E33" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3753,16 +3777,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -3775,16 +3799,16 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -3797,16 +3821,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -3819,16 +3843,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -3841,16 +3865,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -3863,16 +3887,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -3885,16 +3909,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -3907,16 +3931,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -3929,16 +3953,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -3951,16 +3975,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -3973,15 +3997,15 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="21" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="23" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -4166,36 +4190,38 @@
     <hyperlink ref="D13" r:id="rId4"/>
     <hyperlink ref="D14" r:id="rId5"/>
     <hyperlink ref="D15" r:id="rId6"/>
-    <hyperlink ref="D17" r:id="rId7"/>
-    <hyperlink ref="D18" r:id="rId8"/>
-    <hyperlink ref="D19" r:id="rId9"/>
-    <hyperlink ref="D20" r:id="rId10"/>
-    <hyperlink ref="D21" r:id="rId11"/>
-    <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D23" r:id="rId13"/>
-    <hyperlink ref="D24" r:id="rId14"/>
-    <hyperlink ref="D25" r:id="rId15"/>
-    <hyperlink ref="D26" r:id="rId16"/>
-    <hyperlink ref="D28" r:id="rId17"/>
-    <hyperlink ref="D29" r:id="rId18"/>
-    <hyperlink ref="D30" r:id="rId19"/>
-    <hyperlink ref="D31" r:id="rId20"/>
-    <hyperlink ref="D32" r:id="rId21"/>
-    <hyperlink ref="D33" r:id="rId22"/>
-    <hyperlink ref="D34" r:id="rId23"/>
-    <hyperlink ref="D35" r:id="rId24"/>
-    <hyperlink ref="D36" r:id="rId25"/>
-    <hyperlink ref="D37" r:id="rId26"/>
-    <hyperlink ref="D38" r:id="rId27"/>
-    <hyperlink ref="D39" r:id="rId28"/>
-    <hyperlink ref="D40" r:id="rId29"/>
-    <hyperlink ref="D41" r:id="rId30"/>
-    <hyperlink ref="D42" r:id="rId31"/>
-    <hyperlink ref="D43" r:id="rId32"/>
+    <hyperlink ref="D16" r:id="rId7"/>
+    <hyperlink ref="D17" r:id="rId8"/>
+    <hyperlink ref="D18" r:id="rId9"/>
+    <hyperlink ref="D19" r:id="rId10"/>
+    <hyperlink ref="D20" r:id="rId11"/>
+    <hyperlink ref="D21" r:id="rId12"/>
+    <hyperlink ref="D22" r:id="rId13"/>
+    <hyperlink ref="D23" r:id="rId14"/>
+    <hyperlink ref="D24" r:id="rId15"/>
+    <hyperlink ref="D25" r:id="rId16"/>
+    <hyperlink ref="D26" r:id="rId17"/>
+    <hyperlink ref="D27" r:id="rId18"/>
+    <hyperlink ref="D28" r:id="rId19"/>
+    <hyperlink ref="D29" r:id="rId20"/>
+    <hyperlink ref="D30" r:id="rId21"/>
+    <hyperlink ref="D31" r:id="rId22"/>
+    <hyperlink ref="D32" r:id="rId23"/>
+    <hyperlink ref="D33" r:id="rId24"/>
+    <hyperlink ref="D34" r:id="rId25"/>
+    <hyperlink ref="D35" r:id="rId26"/>
+    <hyperlink ref="D36" r:id="rId27"/>
+    <hyperlink ref="D37" r:id="rId28"/>
+    <hyperlink ref="D38" r:id="rId29"/>
+    <hyperlink ref="D39" r:id="rId30"/>
+    <hyperlink ref="D40" r:id="rId31"/>
+    <hyperlink ref="D41" r:id="rId32"/>
+    <hyperlink ref="D42" r:id="rId33"/>
+    <hyperlink ref="D43" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId33"/>
-  <legacyDrawing r:id="rId34"/>
+  <drawing r:id="rId35"/>
+  <legacyDrawing r:id="rId36"/>
 </worksheet>
 </file>
 
@@ -4212,72 +4238,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@b50114df462e431f5aad7a325461e2250139b787 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="275">
   <si>
     <t>Row</t>
   </si>
@@ -373,6 +373,21 @@
     <t>9</t>
   </si>
   <si>
+    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x01</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
   </si>
   <si>
@@ -391,6 +406,9 @@
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>expansion header for Raspberry Pi 2 &amp; 3</t>
   </si>
   <si>
@@ -412,9 +430,6 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -436,6 +451,9 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
   </si>
   <si>
@@ -457,7 +475,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
@@ -481,7 +499,7 @@
     <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x02, script generated</t>
@@ -505,7 +523,7 @@
     <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x03, script generated</t>
@@ -529,7 +547,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>J7</t>
@@ -547,7 +565,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>USB Type A connector</t>
@@ -568,7 +586,7 @@
     <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>Inductor</t>
@@ -592,7 +610,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/7447471022/2794428</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>Inductor with ferrite core</t>
@@ -616,7 +634,7 @@
     <t>https://www.digikey.ch/en/products/detail/fair-rite-products-corp/2743005111/8599429</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>PDQE15-Q24-S5-D</t>
@@ -634,7 +652,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -655,7 +673,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C100J/13537327</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>R3</t>
@@ -667,7 +685,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C330J/13537493</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>R1</t>
@@ -679,7 +697,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C221J/13537314</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>R2 R5</t>
@@ -691,7 +709,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C471J/13537235</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -715,7 +733,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430466043726/5209037</t>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>SW5</t>
@@ -724,19 +742,19 @@
     <t>B</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>SW6</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>SW1</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>SW2</t>
@@ -745,7 +763,7 @@
     <t>E</t>
   </si>
   <si>
-    <t>30</t>
+    <t>31</t>
   </si>
   <si>
     <t>SW3</t>
@@ -754,7 +772,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>31</t>
+    <t>32</t>
   </si>
   <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
@@ -778,15 +796,15 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>SW7</t>
   </si>
   <si>
     <t>VOL Rotary</t>
   </si>
   <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
   </si>
   <si>
@@ -805,7 +823,7 @@
     <t>https://www.digikey.ch/de/products/detail/onsemi/H11L1M/284866</t>
   </si>
   <si>
-    <t>34</t>
+    <t>35</t>
   </si>
   <si>
     <t>Pico</t>
@@ -862,7 +880,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>69 (0 SMD/ 67 THT)</t>
+    <t>70 (0 SMD/ 68 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -901,7 +919,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-26 23:14:44</t>
+    <t>2023-03-27 13:56:09</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
@@ -1676,7 +1694,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1701,7 +1719,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1715,55 +1733,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="F2" s="3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1771,16 +1789,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="F6" s="3">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2125,7 +2143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30" customHeight="1">
+    <row r="17" spans="1:12" ht="60" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
@@ -2139,22 +2157,22 @@
         <v>79</v>
       </c>
       <c r="E17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="G17" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>82</v>
+      <c r="I17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>22</v>
@@ -2168,57 +2186,57 @@
         <v>58</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>87</v>
-      </c>
       <c r="G18" s="9" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="B19" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="60" customHeight="1">
-      <c r="A19" s="5" t="s">
+      <c r="C19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>12</v>
@@ -2227,10 +2245,10 @@
         <v>19</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>22</v>
@@ -2239,36 +2257,36 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="30" customHeight="1">
+    <row r="20" spans="1:12" ht="60" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>102</v>
-      </c>
       <c r="G20" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>22</v>
@@ -2279,22 +2297,22 @@
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>18</v>
@@ -2303,10 +2321,10 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>22</v>
@@ -2317,34 +2335,34 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="D22" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="G22" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>22</v>
@@ -2355,22 +2373,22 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>126</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>12</v>
@@ -2379,10 +2397,10 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>22</v>
@@ -2393,13 +2411,13 @@
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>84</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>130</v>
@@ -2434,19 +2452,19 @@
         <v>135</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>137</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>12</v>
@@ -2455,10 +2473,10 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>22</v>
@@ -2469,22 +2487,22 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>12</v>
@@ -2493,10 +2511,10 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>22</v>
@@ -2507,34 +2525,34 @@
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="D27" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>155</v>
-      </c>
       <c r="G27" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>22</v>
@@ -2545,25 +2563,25 @@
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>160</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>161</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>19</v>
@@ -2585,20 +2603,20 @@
       <c r="A29" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>168</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
@@ -2607,10 +2625,10 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>22</v>
@@ -2621,22 +2639,22 @@
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>165</v>
-      </c>
       <c r="C30" s="11" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>173</v>
+        <v>58</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>12</v>
@@ -2645,10 +2663,10 @@
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>22</v>
@@ -2659,22 +2677,22 @@
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>12</v>
@@ -2683,10 +2701,10 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>22</v>
@@ -2697,34 +2715,34 @@
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>22</v>
@@ -2735,13 +2753,13 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>186</v>
@@ -2750,19 +2768,19 @@
         <v>187</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>22</v>
@@ -2773,13 +2791,13 @@
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>191</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>192</v>
@@ -2788,7 +2806,7 @@
         <v>193</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>12</v>
@@ -2797,10 +2815,10 @@
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>22</v>
@@ -2811,22 +2829,22 @@
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
@@ -2835,10 +2853,10 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>22</v>
@@ -2849,22 +2867,22 @@
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>12</v>
@@ -2873,10 +2891,10 @@
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>22</v>
@@ -2887,22 +2905,22 @@
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
@@ -2911,10 +2929,10 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>22</v>
@@ -2925,22 +2943,22 @@
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -2949,10 +2967,10 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>22</v>
@@ -2963,22 +2981,22 @@
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -2987,10 +3005,10 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>22</v>
@@ -3001,13 +3019,13 @@
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>206</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>213</v>
@@ -3016,7 +3034,7 @@
         <v>214</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3025,10 +3043,10 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>22</v>
@@ -3039,22 +3057,22 @@
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="F41" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>218</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3063,10 +3081,10 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>22</v>
@@ -3077,10 +3095,10 @@
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>22</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>222</v>
@@ -3110,6 +3128,44 @@
         <v>22</v>
       </c>
       <c r="L42" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="30" customHeight="1">
+      <c r="A43" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3125,7 +3181,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -3147,7 +3203,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3155,13 +3211,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3169,13 +3225,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3184,38 +3240,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G43)</f>
+        <f>SUM(G10:G44)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3235,16 +3291,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3423,22 +3479,19 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1">
+    <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
         <v>79</v>
       </c>
       <c r="B18" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>82</v>
-      </c>
       <c r="E18" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G18" s="20">
         <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
@@ -3447,20 +3500,20 @@
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>88</v>
-      </c>
       <c r="E19" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
@@ -3469,16 +3522,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>94</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -3489,22 +3542,22 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>103</v>
-      </c>
       <c r="E21" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
@@ -3513,16 +3566,16 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>109</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>111</v>
       </c>
       <c r="E22" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3533,22 +3586,22 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>119</v>
-      </c>
       <c r="E23" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -3557,16 +3610,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>127</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -3577,7 +3630,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
         <v>130</v>
       </c>
@@ -3599,18 +3652,18 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>137</v>
       </c>
       <c r="C26" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="19" t="s">
         <v>139</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>140</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -3623,16 +3676,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="D27" s="19" t="s">
         <v>146</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>148</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -3645,32 +3698,32 @@
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C28" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>156</v>
-      </c>
       <c r="E28" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G28" s="20">
         <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>160</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>159</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>161</v>
@@ -3679,8 +3732,8 @@
         <v>162</v>
       </c>
       <c r="E29" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>
@@ -3689,16 +3742,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>168</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>169</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -3711,16 +3764,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>173</v>
+        <v>58</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -3733,16 +3786,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -3755,27 +3808,27 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E33" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G33" s="20">
         <f>IF(AND(ISNUMBER(E33),ISNUMBER(F33)),E33*F33,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1">
+    <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
         <v>186</v>
       </c>
@@ -3783,14 +3836,14 @@
         <v>187</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="E34" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G34" s="20">
         <f>IF(AND(ISNUMBER(E34),ISNUMBER(F34)),E34*F34,"")</f>
@@ -3805,10 +3858,10 @@
         <v>193</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -3821,16 +3874,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>195</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>189</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -3843,16 +3896,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -3865,16 +3918,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -3887,16 +3940,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -3909,16 +3962,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -3937,10 +3990,10 @@
         <v>214</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -3953,16 +4006,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B42" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>216</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>219</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -3995,17 +4048,39 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="21" t="s">
-        <v>252</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>253</v>
+    <row r="44" spans="1:7" ht="30" customHeight="1">
+      <c r="A44" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="E44" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G44" s="20">
+        <f>IF(AND(ISNUMBER(E44),ISNUMBER(F44)),E44*F44,"")</f>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="23" t="s">
-        <v>254</v>
+      <c r="A47" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="23" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -4183,6 +4258,11 @@
       <formula>AND(ISBLANK(D43),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="expression" dxfId="0" priority="35">
+      <formula>AND(ISBLANK(D44),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -4192,32 +4272,32 @@
     <hyperlink ref="D15" r:id="rId6"/>
     <hyperlink ref="D16" r:id="rId7"/>
     <hyperlink ref="D17" r:id="rId8"/>
-    <hyperlink ref="D18" r:id="rId9"/>
-    <hyperlink ref="D19" r:id="rId10"/>
-    <hyperlink ref="D20" r:id="rId11"/>
-    <hyperlink ref="D21" r:id="rId12"/>
-    <hyperlink ref="D22" r:id="rId13"/>
-    <hyperlink ref="D23" r:id="rId14"/>
-    <hyperlink ref="D24" r:id="rId15"/>
-    <hyperlink ref="D25" r:id="rId16"/>
-    <hyperlink ref="D26" r:id="rId17"/>
-    <hyperlink ref="D27" r:id="rId18"/>
-    <hyperlink ref="D28" r:id="rId19"/>
-    <hyperlink ref="D29" r:id="rId20"/>
-    <hyperlink ref="D30" r:id="rId21"/>
-    <hyperlink ref="D31" r:id="rId22"/>
-    <hyperlink ref="D32" r:id="rId23"/>
-    <hyperlink ref="D33" r:id="rId24"/>
-    <hyperlink ref="D34" r:id="rId25"/>
-    <hyperlink ref="D35" r:id="rId26"/>
-    <hyperlink ref="D36" r:id="rId27"/>
-    <hyperlink ref="D37" r:id="rId28"/>
-    <hyperlink ref="D38" r:id="rId29"/>
-    <hyperlink ref="D39" r:id="rId30"/>
-    <hyperlink ref="D40" r:id="rId31"/>
-    <hyperlink ref="D41" r:id="rId32"/>
-    <hyperlink ref="D42" r:id="rId33"/>
-    <hyperlink ref="D43" r:id="rId34"/>
+    <hyperlink ref="D19" r:id="rId9"/>
+    <hyperlink ref="D20" r:id="rId10"/>
+    <hyperlink ref="D21" r:id="rId11"/>
+    <hyperlink ref="D22" r:id="rId12"/>
+    <hyperlink ref="D23" r:id="rId13"/>
+    <hyperlink ref="D24" r:id="rId14"/>
+    <hyperlink ref="D25" r:id="rId15"/>
+    <hyperlink ref="D26" r:id="rId16"/>
+    <hyperlink ref="D27" r:id="rId17"/>
+    <hyperlink ref="D28" r:id="rId18"/>
+    <hyperlink ref="D29" r:id="rId19"/>
+    <hyperlink ref="D30" r:id="rId20"/>
+    <hyperlink ref="D31" r:id="rId21"/>
+    <hyperlink ref="D32" r:id="rId22"/>
+    <hyperlink ref="D33" r:id="rId23"/>
+    <hyperlink ref="D34" r:id="rId24"/>
+    <hyperlink ref="D35" r:id="rId25"/>
+    <hyperlink ref="D36" r:id="rId26"/>
+    <hyperlink ref="D37" r:id="rId27"/>
+    <hyperlink ref="D38" r:id="rId28"/>
+    <hyperlink ref="D39" r:id="rId29"/>
+    <hyperlink ref="D40" r:id="rId30"/>
+    <hyperlink ref="D41" r:id="rId31"/>
+    <hyperlink ref="D42" r:id="rId32"/>
+    <hyperlink ref="D43" r:id="rId33"/>
+    <hyperlink ref="D44" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId35"/>
@@ -4238,72 +4318,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@db5d59866f92e973602bd13b33e3b662fc3cce74 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="275">
   <si>
     <t>Row</t>
   </si>
@@ -352,22 +352,25 @@
     <t>8</t>
   </si>
   <si>
-    <t>DC Barrel Jack with a mounting pin</t>
+    <t>DC Barrel Jack with an internal switch</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_Switch</t>
+  </si>
+  <si>
+    <t>J13</t>
   </si>
   <si>
     <t>Barrel_Jack_MountingPin</t>
   </si>
   <si>
-    <t>J13</t>
-  </si>
-  <si>
-    <t>BarrelJack_CUI_PJ-063AH_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/pj-063ah.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/PJ-063AH/2161208</t>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
   <si>
     <t>9</t>
@@ -385,9 +388,6 @@
     <t>PinHeader_1x02_P2.54mm_Horizontal</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
   </si>
   <si>
@@ -919,7 +919,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-27 14:31:33</t>
+    <t>2023-03-27 15:02:34</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
@@ -1705,7 +1705,7 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="60.7109375" customWidth="1"/>
@@ -2119,10 +2119,10 @@
         <v>72</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>12</v>
@@ -2130,11 +2130,11 @@
       <c r="H16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="11" t="s">
-        <v>74</v>
+      <c r="I16" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>22</v>
@@ -2145,22 +2145,22 @@
     </row>
     <row r="17" spans="1:12" ht="60" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="F17" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>12</v>
@@ -2169,7 +2169,7 @@
         <v>19</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>22</v>
@@ -3462,12 +3462,9 @@
         <v>72</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="19" t="s">
         <v>74</v>
       </c>
       <c r="E17" s="19">
@@ -3481,13 +3478,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>78</v>
-      </c>
       <c r="C18" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -4271,37 +4268,36 @@
     <hyperlink ref="D14" r:id="rId5"/>
     <hyperlink ref="D15" r:id="rId6"/>
     <hyperlink ref="D16" r:id="rId7"/>
-    <hyperlink ref="D17" r:id="rId8"/>
-    <hyperlink ref="D19" r:id="rId9"/>
-    <hyperlink ref="D20" r:id="rId10"/>
-    <hyperlink ref="D21" r:id="rId11"/>
-    <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D23" r:id="rId13"/>
-    <hyperlink ref="D24" r:id="rId14"/>
-    <hyperlink ref="D25" r:id="rId15"/>
-    <hyperlink ref="D26" r:id="rId16"/>
-    <hyperlink ref="D27" r:id="rId17"/>
-    <hyperlink ref="D28" r:id="rId18"/>
-    <hyperlink ref="D29" r:id="rId19"/>
-    <hyperlink ref="D30" r:id="rId20"/>
-    <hyperlink ref="D31" r:id="rId21"/>
-    <hyperlink ref="D32" r:id="rId22"/>
-    <hyperlink ref="D33" r:id="rId23"/>
-    <hyperlink ref="D34" r:id="rId24"/>
-    <hyperlink ref="D35" r:id="rId25"/>
-    <hyperlink ref="D36" r:id="rId26"/>
-    <hyperlink ref="D37" r:id="rId27"/>
-    <hyperlink ref="D38" r:id="rId28"/>
-    <hyperlink ref="D39" r:id="rId29"/>
-    <hyperlink ref="D40" r:id="rId30"/>
-    <hyperlink ref="D41" r:id="rId31"/>
-    <hyperlink ref="D42" r:id="rId32"/>
-    <hyperlink ref="D43" r:id="rId33"/>
-    <hyperlink ref="D44" r:id="rId34"/>
+    <hyperlink ref="D19" r:id="rId8"/>
+    <hyperlink ref="D20" r:id="rId9"/>
+    <hyperlink ref="D21" r:id="rId10"/>
+    <hyperlink ref="D22" r:id="rId11"/>
+    <hyperlink ref="D23" r:id="rId12"/>
+    <hyperlink ref="D24" r:id="rId13"/>
+    <hyperlink ref="D25" r:id="rId14"/>
+    <hyperlink ref="D26" r:id="rId15"/>
+    <hyperlink ref="D27" r:id="rId16"/>
+    <hyperlink ref="D28" r:id="rId17"/>
+    <hyperlink ref="D29" r:id="rId18"/>
+    <hyperlink ref="D30" r:id="rId19"/>
+    <hyperlink ref="D31" r:id="rId20"/>
+    <hyperlink ref="D32" r:id="rId21"/>
+    <hyperlink ref="D33" r:id="rId22"/>
+    <hyperlink ref="D34" r:id="rId23"/>
+    <hyperlink ref="D35" r:id="rId24"/>
+    <hyperlink ref="D36" r:id="rId25"/>
+    <hyperlink ref="D37" r:id="rId26"/>
+    <hyperlink ref="D38" r:id="rId27"/>
+    <hyperlink ref="D39" r:id="rId28"/>
+    <hyperlink ref="D40" r:id="rId29"/>
+    <hyperlink ref="D41" r:id="rId30"/>
+    <hyperlink ref="D42" r:id="rId31"/>
+    <hyperlink ref="D43" r:id="rId32"/>
+    <hyperlink ref="D44" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId35"/>
-  <legacyDrawing r:id="rId36"/>
+  <drawing r:id="rId34"/>
+  <legacyDrawing r:id="rId35"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@036b89f8aa95cc76506a1c4ec3cc837328a9c6e6 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="276">
   <si>
     <t>Row</t>
   </si>
@@ -367,27 +367,30 @@
     <t>BarrelJack_Wuerth_6941xx301002</t>
   </si>
   <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x01</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
+  </si>
+  <si>
     <t>~</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x01</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
-  </si>
-  <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
   </si>
   <si>
@@ -919,7 +922,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-27 15:08:04</t>
+    <t>2023-03-27 15:37:32</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
@@ -1719,7 +1722,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1733,13 +1736,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F2" s="3">
         <v>35</v>
@@ -1747,41 +1750,41 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1789,13 +1792,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F6" s="3">
         <v>70</v>
@@ -2130,7 +2133,7 @@
       <c r="H16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>75</v>
       </c>
       <c r="J16" s="10" t="s">
@@ -2169,7 +2172,7 @@
         <v>19</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>22</v>
@@ -2186,19 +2189,19 @@
         <v>58</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>43</v>
@@ -2207,10 +2210,10 @@
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>22</v>
@@ -2221,22 +2224,22 @@
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>12</v>
@@ -2245,10 +2248,10 @@
         <v>19</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>22</v>
@@ -2262,19 +2265,19 @@
         <v>26</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>12</v>
@@ -2283,10 +2286,10 @@
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>22</v>
@@ -2297,22 +2300,22 @@
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>18</v>
@@ -2321,10 +2324,10 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>22</v>
@@ -2335,22 +2338,22 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>18</v>
@@ -2359,10 +2362,10 @@
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>22</v>
@@ -2373,22 +2376,22 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>12</v>
@@ -2397,10 +2400,10 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>22</v>
@@ -2411,22 +2414,22 @@
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>12</v>
@@ -2435,10 +2438,10 @@
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>22</v>
@@ -2449,22 +2452,22 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>12</v>
@@ -2473,10 +2476,10 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>22</v>
@@ -2487,22 +2490,22 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D26" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>143</v>
-      </c>
       <c r="F26" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>12</v>
@@ -2511,10 +2514,10 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>22</v>
@@ -2525,22 +2528,22 @@
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>12</v>
@@ -2549,10 +2552,10 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>22</v>
@@ -2563,22 +2566,22 @@
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>43</v>
@@ -2587,10 +2590,10 @@
         <v>19</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>22</v>
@@ -2601,22 +2604,22 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>165</v>
-      </c>
       <c r="F29" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
@@ -2625,10 +2628,10 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>22</v>
@@ -2639,22 +2642,22 @@
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>12</v>
@@ -2663,10 +2666,10 @@
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>22</v>
@@ -2677,22 +2680,22 @@
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>12</v>
@@ -2701,10 +2704,10 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>22</v>
@@ -2715,22 +2718,22 @@
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>12</v>
@@ -2739,10 +2742,10 @@
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>22</v>
@@ -2753,22 +2756,22 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>18</v>
@@ -2777,10 +2780,10 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>22</v>
@@ -2791,22 +2794,22 @@
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>12</v>
@@ -2815,10 +2818,10 @@
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>22</v>
@@ -2829,22 +2832,22 @@
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
@@ -2853,10 +2856,10 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>22</v>
@@ -2867,22 +2870,22 @@
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>12</v>
@@ -2891,10 +2894,10 @@
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>22</v>
@@ -2905,22 +2908,22 @@
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
@@ -2929,10 +2932,10 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>22</v>
@@ -2943,22 +2946,22 @@
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -2967,10 +2970,10 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>22</v>
@@ -2981,22 +2984,22 @@
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -3005,10 +3008,10 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>22</v>
@@ -3019,22 +3022,22 @@
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3043,10 +3046,10 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>22</v>
@@ -3057,22 +3060,22 @@
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3081,10 +3084,10 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>22</v>
@@ -3095,22 +3098,22 @@
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D42" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>222</v>
-      </c>
       <c r="F42" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>12</v>
@@ -3119,10 +3122,10 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>22</v>
@@ -3133,22 +3136,22 @@
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D43" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>228</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>12</v>
@@ -3157,10 +3160,10 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>22</v>
@@ -3203,7 +3206,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3211,13 +3214,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3225,13 +3228,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3240,13 +3243,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G44)</f>
@@ -3255,23 +3258,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3291,16 +3294,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3457,7 +3460,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="19" t="s">
         <v>72</v>
       </c>
@@ -3466,6 +3469,9 @@
       </c>
       <c r="C17" s="19" t="s">
         <v>74</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -3497,16 +3503,16 @@
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E19" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -3519,16 +3525,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -3541,16 +3547,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E21" s="19">
         <f>BoardQty*1</f>
@@ -3563,16 +3569,16 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E22" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3585,16 +3591,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3607,16 +3613,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -3629,16 +3635,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -3651,16 +3657,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -3673,16 +3679,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>143</v>
-      </c>
       <c r="C27" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -3695,16 +3701,16 @@
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -3717,16 +3723,16 @@
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -3739,16 +3745,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>165</v>
-      </c>
       <c r="C30" s="19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -3761,16 +3767,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -3783,16 +3789,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -3805,16 +3811,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -3827,16 +3833,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3849,16 +3855,16 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -3871,16 +3877,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -3893,16 +3899,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -3915,16 +3921,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -3937,16 +3943,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -3959,16 +3965,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -3981,16 +3987,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4003,16 +4009,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4025,16 +4031,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>222</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4047,16 +4053,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>228</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4069,15 +4075,15 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="21" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="23" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -4268,36 +4274,37 @@
     <hyperlink ref="D14" r:id="rId5"/>
     <hyperlink ref="D15" r:id="rId6"/>
     <hyperlink ref="D16" r:id="rId7"/>
-    <hyperlink ref="D19" r:id="rId8"/>
-    <hyperlink ref="D20" r:id="rId9"/>
-    <hyperlink ref="D21" r:id="rId10"/>
-    <hyperlink ref="D22" r:id="rId11"/>
-    <hyperlink ref="D23" r:id="rId12"/>
-    <hyperlink ref="D24" r:id="rId13"/>
-    <hyperlink ref="D25" r:id="rId14"/>
-    <hyperlink ref="D26" r:id="rId15"/>
-    <hyperlink ref="D27" r:id="rId16"/>
-    <hyperlink ref="D28" r:id="rId17"/>
-    <hyperlink ref="D29" r:id="rId18"/>
-    <hyperlink ref="D30" r:id="rId19"/>
-    <hyperlink ref="D31" r:id="rId20"/>
-    <hyperlink ref="D32" r:id="rId21"/>
-    <hyperlink ref="D33" r:id="rId22"/>
-    <hyperlink ref="D34" r:id="rId23"/>
-    <hyperlink ref="D35" r:id="rId24"/>
-    <hyperlink ref="D36" r:id="rId25"/>
-    <hyperlink ref="D37" r:id="rId26"/>
-    <hyperlink ref="D38" r:id="rId27"/>
-    <hyperlink ref="D39" r:id="rId28"/>
-    <hyperlink ref="D40" r:id="rId29"/>
-    <hyperlink ref="D41" r:id="rId30"/>
-    <hyperlink ref="D42" r:id="rId31"/>
-    <hyperlink ref="D43" r:id="rId32"/>
-    <hyperlink ref="D44" r:id="rId33"/>
+    <hyperlink ref="D17" r:id="rId8"/>
+    <hyperlink ref="D19" r:id="rId9"/>
+    <hyperlink ref="D20" r:id="rId10"/>
+    <hyperlink ref="D21" r:id="rId11"/>
+    <hyperlink ref="D22" r:id="rId12"/>
+    <hyperlink ref="D23" r:id="rId13"/>
+    <hyperlink ref="D24" r:id="rId14"/>
+    <hyperlink ref="D25" r:id="rId15"/>
+    <hyperlink ref="D26" r:id="rId16"/>
+    <hyperlink ref="D27" r:id="rId17"/>
+    <hyperlink ref="D28" r:id="rId18"/>
+    <hyperlink ref="D29" r:id="rId19"/>
+    <hyperlink ref="D30" r:id="rId20"/>
+    <hyperlink ref="D31" r:id="rId21"/>
+    <hyperlink ref="D32" r:id="rId22"/>
+    <hyperlink ref="D33" r:id="rId23"/>
+    <hyperlink ref="D34" r:id="rId24"/>
+    <hyperlink ref="D35" r:id="rId25"/>
+    <hyperlink ref="D36" r:id="rId26"/>
+    <hyperlink ref="D37" r:id="rId27"/>
+    <hyperlink ref="D38" r:id="rId28"/>
+    <hyperlink ref="D39" r:id="rId29"/>
+    <hyperlink ref="D40" r:id="rId30"/>
+    <hyperlink ref="D41" r:id="rId31"/>
+    <hyperlink ref="D42" r:id="rId32"/>
+    <hyperlink ref="D43" r:id="rId33"/>
+    <hyperlink ref="D44" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId34"/>
-  <legacyDrawing r:id="rId35"/>
+  <drawing r:id="rId35"/>
+  <legacyDrawing r:id="rId36"/>
 </worksheet>
 </file>
 
@@ -4314,72 +4321,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@bc3196ee1f2e587f970f960ee2b963110b6337e8 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -235,7 +235,7 @@
     <t>C16 C17</t>
   </si>
   <si>
-    <t>4.7uF 50V</t>
+    <t>4.7uF</t>
   </si>
   <si>
     <t>C_Disc_D5.1mm_W3.2mm_P5.00mm</t>
@@ -625,7 +625,7 @@
     <t>L1 L2 L3 L4 L5</t>
   </si>
   <si>
-    <t>1K@100MHz</t>
+    <t>103_100MHz</t>
   </si>
   <si>
     <t>L_Axial_L6.6mm_D2.7mm_P10.16mm_Horizontal_Vishay_IM-2</t>
@@ -922,7 +922,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-27 15:39:50</t>
+    <t>2023-03-27 17:01:24</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@6341635dc6f0f093d687465be6828836a169a0a5 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="277">
   <si>
     <t>Row</t>
   </si>
@@ -388,7 +388,10 @@
     <t>PinHeader_1x02_P2.54mm_Horizontal</t>
   </si>
   <si>
-    <t>~</t>
+    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
   </si>
   <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
@@ -922,7 +925,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-27 18:59:40</t>
+    <t>2023-03-27 19:26:08</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
@@ -1722,7 +1725,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1736,13 +1739,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F2" s="3">
         <v>35</v>
@@ -1750,41 +1753,41 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1792,13 +1795,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F6" s="3">
         <v>70</v>
@@ -2171,11 +2174,11 @@
       <c r="H17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>22</v>
+      <c r="J17" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>22</v>
@@ -2189,19 +2192,19 @@
         <v>58</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>43</v>
@@ -2210,10 +2213,10 @@
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>22</v>
@@ -2224,22 +2227,22 @@
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>12</v>
@@ -2248,10 +2251,10 @@
         <v>19</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>22</v>
@@ -2265,19 +2268,19 @@
         <v>26</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>12</v>
@@ -2286,10 +2289,10 @@
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>22</v>
@@ -2300,22 +2303,22 @@
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>18</v>
@@ -2324,10 +2327,10 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>22</v>
@@ -2338,22 +2341,22 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>18</v>
@@ -2362,10 +2365,10 @@
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>22</v>
@@ -2376,22 +2379,22 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>12</v>
@@ -2400,10 +2403,10 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>22</v>
@@ -2414,22 +2417,22 @@
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>12</v>
@@ -2438,10 +2441,10 @@
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>22</v>
@@ -2452,22 +2455,22 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>12</v>
@@ -2476,10 +2479,10 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>22</v>
@@ -2490,22 +2493,22 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D26" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>144</v>
-      </c>
       <c r="F26" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>12</v>
@@ -2514,10 +2517,10 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>22</v>
@@ -2528,22 +2531,22 @@
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>12</v>
@@ -2552,10 +2555,10 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>22</v>
@@ -2566,22 +2569,22 @@
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>43</v>
@@ -2590,10 +2593,10 @@
         <v>19</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>22</v>
@@ -2604,22 +2607,22 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>166</v>
-      </c>
       <c r="F29" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
@@ -2628,10 +2631,10 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>22</v>
@@ -2642,22 +2645,22 @@
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>12</v>
@@ -2666,10 +2669,10 @@
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>22</v>
@@ -2680,22 +2683,22 @@
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>12</v>
@@ -2704,10 +2707,10 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>22</v>
@@ -2718,22 +2721,22 @@
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>12</v>
@@ -2742,10 +2745,10 @@
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>22</v>
@@ -2756,22 +2759,22 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>18</v>
@@ -2780,10 +2783,10 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>22</v>
@@ -2794,22 +2797,22 @@
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>12</v>
@@ -2818,10 +2821,10 @@
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>22</v>
@@ -2832,22 +2835,22 @@
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
@@ -2856,10 +2859,10 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>22</v>
@@ -2870,22 +2873,22 @@
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>12</v>
@@ -2894,10 +2897,10 @@
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>22</v>
@@ -2908,22 +2911,22 @@
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
@@ -2932,10 +2935,10 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>22</v>
@@ -2946,22 +2949,22 @@
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -2970,10 +2973,10 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>22</v>
@@ -2984,22 +2987,22 @@
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -3008,10 +3011,10 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>22</v>
@@ -3022,22 +3025,22 @@
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3046,10 +3049,10 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>22</v>
@@ -3060,22 +3063,22 @@
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3084,10 +3087,10 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>22</v>
@@ -3098,22 +3101,22 @@
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D42" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>223</v>
-      </c>
       <c r="F42" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>12</v>
@@ -3122,10 +3125,10 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>22</v>
@@ -3136,22 +3139,22 @@
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D43" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>229</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>12</v>
@@ -3160,10 +3163,10 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>22</v>
@@ -3206,7 +3209,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3214,13 +3217,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3228,13 +3231,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3243,13 +3246,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G44)</f>
@@ -3258,23 +3261,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3294,16 +3297,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3482,7 +3485,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="30" customHeight="1">
       <c r="A18" s="19" t="s">
         <v>80</v>
       </c>
@@ -3491,6 +3494,9 @@
       </c>
       <c r="C18" s="19" t="s">
         <v>81</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -3503,16 +3509,16 @@
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E19" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -3525,16 +3531,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -3547,16 +3553,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E21" s="19">
         <f>BoardQty*1</f>
@@ -3569,16 +3575,16 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E22" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3591,16 +3597,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3613,16 +3619,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -3635,16 +3641,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -3657,16 +3663,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -3679,16 +3685,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>144</v>
-      </c>
       <c r="C27" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -3701,16 +3707,16 @@
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -3723,16 +3729,16 @@
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -3745,16 +3751,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>166</v>
-      </c>
       <c r="C30" s="19" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -3767,16 +3773,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -3789,16 +3795,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -3811,16 +3817,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -3833,16 +3839,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3855,16 +3861,16 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -3877,16 +3883,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -3899,16 +3905,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -3921,16 +3927,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -3943,16 +3949,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -3965,16 +3971,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -3987,16 +3993,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4009,16 +4015,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4031,16 +4037,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>223</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4053,16 +4059,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>229</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4075,15 +4081,15 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="23" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -4275,36 +4281,37 @@
     <hyperlink ref="D15" r:id="rId6"/>
     <hyperlink ref="D16" r:id="rId7"/>
     <hyperlink ref="D17" r:id="rId8"/>
-    <hyperlink ref="D19" r:id="rId9"/>
-    <hyperlink ref="D20" r:id="rId10"/>
-    <hyperlink ref="D21" r:id="rId11"/>
-    <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D23" r:id="rId13"/>
-    <hyperlink ref="D24" r:id="rId14"/>
-    <hyperlink ref="D25" r:id="rId15"/>
-    <hyperlink ref="D26" r:id="rId16"/>
-    <hyperlink ref="D27" r:id="rId17"/>
-    <hyperlink ref="D28" r:id="rId18"/>
-    <hyperlink ref="D29" r:id="rId19"/>
-    <hyperlink ref="D30" r:id="rId20"/>
-    <hyperlink ref="D31" r:id="rId21"/>
-    <hyperlink ref="D32" r:id="rId22"/>
-    <hyperlink ref="D33" r:id="rId23"/>
-    <hyperlink ref="D34" r:id="rId24"/>
-    <hyperlink ref="D35" r:id="rId25"/>
-    <hyperlink ref="D36" r:id="rId26"/>
-    <hyperlink ref="D37" r:id="rId27"/>
-    <hyperlink ref="D38" r:id="rId28"/>
-    <hyperlink ref="D39" r:id="rId29"/>
-    <hyperlink ref="D40" r:id="rId30"/>
-    <hyperlink ref="D41" r:id="rId31"/>
-    <hyperlink ref="D42" r:id="rId32"/>
-    <hyperlink ref="D43" r:id="rId33"/>
-    <hyperlink ref="D44" r:id="rId34"/>
+    <hyperlink ref="D18" r:id="rId9"/>
+    <hyperlink ref="D19" r:id="rId10"/>
+    <hyperlink ref="D20" r:id="rId11"/>
+    <hyperlink ref="D21" r:id="rId12"/>
+    <hyperlink ref="D22" r:id="rId13"/>
+    <hyperlink ref="D23" r:id="rId14"/>
+    <hyperlink ref="D24" r:id="rId15"/>
+    <hyperlink ref="D25" r:id="rId16"/>
+    <hyperlink ref="D26" r:id="rId17"/>
+    <hyperlink ref="D27" r:id="rId18"/>
+    <hyperlink ref="D28" r:id="rId19"/>
+    <hyperlink ref="D29" r:id="rId20"/>
+    <hyperlink ref="D30" r:id="rId21"/>
+    <hyperlink ref="D31" r:id="rId22"/>
+    <hyperlink ref="D32" r:id="rId23"/>
+    <hyperlink ref="D33" r:id="rId24"/>
+    <hyperlink ref="D34" r:id="rId25"/>
+    <hyperlink ref="D35" r:id="rId26"/>
+    <hyperlink ref="D36" r:id="rId27"/>
+    <hyperlink ref="D37" r:id="rId28"/>
+    <hyperlink ref="D38" r:id="rId29"/>
+    <hyperlink ref="D39" r:id="rId30"/>
+    <hyperlink ref="D40" r:id="rId31"/>
+    <hyperlink ref="D41" r:id="rId32"/>
+    <hyperlink ref="D42" r:id="rId33"/>
+    <hyperlink ref="D43" r:id="rId34"/>
+    <hyperlink ref="D44" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId35"/>
-  <legacyDrawing r:id="rId36"/>
+  <drawing r:id="rId36"/>
+  <legacyDrawing r:id="rId37"/>
 </worksheet>
 </file>
 
@@ -4321,72 +4328,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@da39d0c479a1802fa2e1b4b9e8f88e25afb93e0b 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -865,7 +865,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>0.0.1</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Date:</t>
@@ -925,7 +925,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-27 19:40:07</t>
+    <t>2023-03-27 20:52:32</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@5c5707f5e27d2ebd435852af6b7c544ce596c50b 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -865,7 +865,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -925,7 +925,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-27 20:52:32</t>
+    <t>2023-03-27 21:24:36</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@7cebe996615351be165b0b955a7aff10b10ae239 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="278">
   <si>
     <t>Row</t>
   </si>
@@ -409,6 +409,9 @@
     <t>Jack_6.35mm_Horizontal</t>
   </si>
   <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
@@ -499,7 +502,7 @@
     <t>CP-2350</t>
   </si>
   <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf?5023</t>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
@@ -925,7 +928,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-03-27 21:35:43</t>
+    <t>2023-03-28 14:07:45</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
@@ -1725,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1739,13 +1742,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F2" s="3">
         <v>35</v>
@@ -1753,41 +1756,41 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1795,13 +1798,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F6" s="3">
         <v>70</v>
@@ -2216,7 +2219,7 @@
         <v>89</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>22</v>
@@ -2227,22 +2230,22 @@
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>12</v>
@@ -2251,10 +2254,10 @@
         <v>19</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>22</v>
@@ -2268,19 +2271,19 @@
         <v>26</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>12</v>
@@ -2289,10 +2292,10 @@
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>22</v>
@@ -2303,22 +2306,22 @@
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>18</v>
@@ -2327,10 +2330,10 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>22</v>
@@ -2341,22 +2344,22 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>18</v>
@@ -2365,10 +2368,10 @@
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>22</v>
@@ -2379,22 +2382,22 @@
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>12</v>
@@ -2403,10 +2406,10 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>22</v>
@@ -2417,22 +2420,22 @@
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>12</v>
@@ -2441,10 +2444,10 @@
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>22</v>
@@ -2455,22 +2458,22 @@
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>12</v>
@@ -2479,10 +2482,10 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>22</v>
@@ -2493,22 +2496,22 @@
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D26" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>145</v>
-      </c>
       <c r="F26" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>12</v>
@@ -2517,10 +2520,10 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K26" s="12" t="s">
         <v>22</v>
@@ -2531,22 +2534,22 @@
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>12</v>
@@ -2555,10 +2558,10 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>22</v>
@@ -2569,22 +2572,22 @@
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>43</v>
@@ -2593,10 +2596,10 @@
         <v>19</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K28" s="12" t="s">
         <v>22</v>
@@ -2607,22 +2610,22 @@
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="F29" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
@@ -2631,10 +2634,10 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>22</v>
@@ -2645,22 +2648,22 @@
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>12</v>
@@ -2669,10 +2672,10 @@
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>22</v>
@@ -2683,22 +2686,22 @@
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>12</v>
@@ -2707,10 +2710,10 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K31" s="8" t="s">
         <v>22</v>
@@ -2721,22 +2724,22 @@
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>12</v>
@@ -2745,10 +2748,10 @@
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K32" s="12" t="s">
         <v>22</v>
@@ -2759,22 +2762,22 @@
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>18</v>
@@ -2783,10 +2786,10 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>22</v>
@@ -2797,22 +2800,22 @@
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>12</v>
@@ -2821,10 +2824,10 @@
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K34" s="12" t="s">
         <v>22</v>
@@ -2835,22 +2838,22 @@
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
@@ -2859,10 +2862,10 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>22</v>
@@ -2873,22 +2876,22 @@
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>12</v>
@@ -2897,10 +2900,10 @@
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K36" s="12" t="s">
         <v>22</v>
@@ -2911,22 +2914,22 @@
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
@@ -2935,10 +2938,10 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K37" s="8" t="s">
         <v>22</v>
@@ -2949,22 +2952,22 @@
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -2973,10 +2976,10 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K38" s="12" t="s">
         <v>22</v>
@@ -2987,22 +2990,22 @@
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -3011,10 +3014,10 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>22</v>
@@ -3025,22 +3028,22 @@
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3049,10 +3052,10 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K40" s="12" t="s">
         <v>22</v>
@@ -3063,22 +3066,22 @@
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3087,10 +3090,10 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>22</v>
@@ -3101,22 +3104,22 @@
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D42" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>224</v>
-      </c>
       <c r="F42" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>12</v>
@@ -3125,10 +3128,10 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="K42" s="12" t="s">
         <v>22</v>
@@ -3139,22 +3142,22 @@
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D43" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>230</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>12</v>
@@ -3163,10 +3166,10 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>22</v>
@@ -3209,7 +3212,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3217,13 +3220,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3231,13 +3234,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3246,13 +3249,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G44)</f>
@@ -3261,23 +3264,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3297,16 +3300,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3507,7 +3510,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1">
+    <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
         <v>86</v>
       </c>
@@ -3531,16 +3534,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -3553,16 +3556,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E21" s="19">
         <f>BoardQty*1</f>
@@ -3575,16 +3578,16 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E22" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3597,16 +3600,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3619,16 +3622,16 @@
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -3641,16 +3644,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -3663,16 +3666,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -3685,16 +3688,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>145</v>
-      </c>
       <c r="C27" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -3707,16 +3710,16 @@
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -3729,16 +3732,16 @@
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E29" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -3751,16 +3754,16 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>167</v>
-      </c>
       <c r="C30" s="19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -3773,16 +3776,16 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -3795,16 +3798,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -3817,16 +3820,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -3839,16 +3842,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E34" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3861,16 +3864,16 @@
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -3883,16 +3886,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -3905,16 +3908,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -3927,16 +3930,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -3949,16 +3952,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -3971,16 +3974,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -3993,16 +3996,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4015,16 +4018,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4037,16 +4040,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>224</v>
-      </c>
       <c r="C43" s="19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4059,16 +4062,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>230</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4081,15 +4084,15 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="21" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="23" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4328,72 +4331,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@c52e15f0cbf7518597d25a415414a62a6e9c8c80 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -868,7 +868,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Date:</t>
@@ -928,7 +928,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-04 14:51:16</t>
+    <t>2023-04-04 15:15:35</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@44edab69321ebbf7135c8c10b86742efa3d222af 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="285">
   <si>
     <t>Row</t>
   </si>
@@ -169,15 +169,15 @@
     <t>Datasheet</t>
   </si>
   <si>
+    <t>Sim.Device</t>
+  </si>
+  <si>
+    <t>Sim.Pins</t>
+  </si>
+  <si>
     <t>Supplier</t>
   </si>
   <si>
-    <t>Sim.Device</t>
-  </si>
-  <si>
-    <t>Sim.Pins</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -205,12 +205,12 @@
     <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/C322C101K1G5TA7301.pdf</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>https://www.digikey.ch/de/products/detail/kemet/C330C102JHR5TA/1465599</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>C1 C2 C3 C4 C5 C6 C7 C8 C9 C10 C11 C12</t>
   </si>
   <si>
@@ -289,18 +289,39 @@
     <t>https://www.onsemi.com/download/data-sheet/pdf/1n914-d.pdf</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>1=K 2=A</t>
+  </si>
+  <si>
     <t>https://www.digikey.ch/en/products/detail/onsemi/1N4148/458603</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>1=K 2=A</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
+    <t>100V 3A General Purpose Rectifier Diode, DO-201AD</t>
+  </si>
+  <si>
+    <t>1N5401</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D_DO-201AD_P15.24mm_Horizontal</t>
+  </si>
+  <si>
+    <t>http://www.vishay.com/docs/88516/1n5400.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/1N5401G/1485525</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>RGB LED with integrated controller, 5mm/8mm LED package</t>
   </si>
   <si>
@@ -325,7 +346,7 @@
     <t>https://www.digikey.ch/de/products/detail/sparkfun-electronics/COM-12986/5673799</t>
   </si>
   <si>
-    <t>7</t>
+    <t>8</t>
   </si>
   <si>
     <t>Resettable fuse, polymeric positive temperature coefficient</t>
@@ -343,13 +364,13 @@
     <t>C_Rect_L7.0mm_W3.5mm_P5.00mm</t>
   </si>
   <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Bel%20Fuse%20PDFs/0ZRP_Series.pdf</t>
+    <t>https://www.onsemi.com/pdf/datasheet/1n5400-d.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/bel-fuse-inc/0ZRP0090FF1E/9468255</t>
   </si>
   <si>
-    <t>8</t>
+    <t>9</t>
   </si>
   <si>
     <t>DC Barrel Jack with an internal switch</t>
@@ -373,9 +394,6 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -394,6 +412,9 @@
     <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
   </si>
   <si>
@@ -415,9 +436,6 @@
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>expansion header for Raspberry Pi 2 &amp; 3</t>
   </si>
   <si>
@@ -439,6 +457,9 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -460,7 +481,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
@@ -484,7 +505,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
@@ -508,7 +529,7 @@
     <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x02, script generated</t>
@@ -532,7 +553,7 @@
     <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x03, script generated</t>
@@ -556,7 +577,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>J7</t>
@@ -574,7 +595,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>USB Type A connector</t>
@@ -595,7 +616,7 @@
     <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>Inductor</t>
@@ -619,7 +640,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/7447471022/2794428</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>Inductor with ferrite core</t>
@@ -643,7 +664,7 @@
     <t>https://www.digikey.ch/en/products/detail/fair-rite-products-corp/2743005111/8599429</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>PDQE15-Q24-S5-D</t>
@@ -661,7 +682,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -682,7 +703,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C100J/13537327</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>R3</t>
@@ -694,7 +715,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C330J/13537493</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>R1</t>
@@ -706,7 +727,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C221J/13537314</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>R2 R5</t>
@@ -718,7 +739,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C471J/13537235</t>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -742,7 +763,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430466043726/5209037</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>SW5</t>
@@ -751,19 +772,19 @@
     <t>B</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>SW6</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>SW1</t>
   </si>
   <si>
-    <t>30</t>
+    <t>31</t>
   </si>
   <si>
     <t>SW2</t>
@@ -772,7 +793,7 @@
     <t>E</t>
   </si>
   <si>
-    <t>31</t>
+    <t>32</t>
   </si>
   <si>
     <t>SW3</t>
@@ -781,9 +802,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
   </si>
   <si>
@@ -805,13 +823,16 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
   </si>
   <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>SW7</t>
   </si>
   <si>
     <t>VOL Rotary</t>
   </si>
   <si>
-    <t>34</t>
+    <t>35</t>
   </si>
   <si>
     <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
@@ -832,7 +853,7 @@
     <t>https://www.digikey.ch/de/products/detail/onsemi/H11L1M/284866</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>Pico</t>
@@ -889,7 +910,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>70 (0 SMD/ 68 THT)</t>
+    <t>71 (0 SMD/ 69 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -928,7 +949,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-06 11:29:01</t>
+    <t>2023-04-07 09:51:47</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
@@ -1703,7 +1724,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1721,14 +1742,14 @@
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
-    <col min="10" max="10" width="60.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1742,55 +1763,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="F2" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1798,16 +1819,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="F6" s="3">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1876,13 +1897,13 @@
       <c r="I9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="8" t="s">
         <v>21</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1914,14 +1935,14 @@
       <c r="I10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
@@ -1952,14 +1973,14 @@
       <c r="I11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
@@ -1990,14 +2011,14 @@
       <c r="I12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
@@ -2052,86 +2073,86 @@
         <v>55</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>57</v>
-      </c>
       <c r="G14" s="9" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>22</v>
+        <v>49</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="G15" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>12</v>
@@ -2140,33 +2161,33 @@
         <v>19</v>
       </c>
       <c r="I16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="10" t="s">
+    </row>
+    <row r="17" spans="1:12" ht="30" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K16" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="60" customHeight="1">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>81</v>
@@ -2180,19 +2201,19 @@
       <c r="I17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
+    </row>
+    <row r="18" spans="1:12" ht="60" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>84</v>
@@ -2204,86 +2225,86 @@
         <v>86</v>
       </c>
       <c r="E18" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>88</v>
-      </c>
       <c r="G18" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I18" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="G19" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="60" customHeight="1">
+    </row>
+    <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>12</v>
@@ -2292,74 +2313,74 @@
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J20" s="10" t="s">
+    </row>
+    <row r="21" spans="1:12" ht="60" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="30" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="G21" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>18</v>
@@ -2368,74 +2389,74 @@
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="G23" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>134</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>12</v>
@@ -2444,36 +2465,36 @@
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="C25" s="7" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>12</v>
@@ -2482,33 +2503,33 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="J25" s="6" t="s">
         <v>143</v>
       </c>
+      <c r="J25" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="K25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>146</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>148</v>
@@ -2522,14 +2543,14 @@
       <c r="I26" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="K26" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
@@ -2546,10 +2567,10 @@
         <v>154</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>12</v>
@@ -2558,62 +2579,62 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="F28" s="11" t="s">
-        <v>164</v>
-      </c>
       <c r="G28" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I28" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>168</v>
@@ -2622,36 +2643,36 @@
         <v>169</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="J29" s="6" t="s">
         <v>172</v>
       </c>
+      <c r="J29" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="K29" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="10" t="s">
         <v>174</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>175</v>
@@ -2660,7 +2681,7 @@
         <v>176</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>58</v>
+        <v>175</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>177</v>
@@ -2674,14 +2695,14 @@
       <c r="I30" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="J30" s="10" t="s">
+      <c r="J30" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="10" t="s">
         <v>179</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
@@ -2689,19 +2710,19 @@
         <v>180</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>12</v>
@@ -2710,36 +2731,36 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>183</v>
+        <v>185</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>12</v>
@@ -2748,112 +2769,112 @@
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L32" s="10" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L34" s="12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>193</v>
-      </c>
       <c r="C35" s="7" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
@@ -2862,36 +2883,36 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>199</v>
+        <v>205</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D36" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>197</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>12</v>
@@ -2900,36 +2921,36 @@
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>199</v>
+        <v>205</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L36" s="10" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
@@ -2938,36 +2959,36 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>199</v>
+        <v>205</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -2976,36 +2997,36 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>199</v>
+        <v>205</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L38" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -3014,36 +3035,36 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>199</v>
+        <v>205</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3052,36 +3073,36 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>220</v>
+        <v>205</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L40" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3090,36 +3111,36 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>220</v>
+        <v>225</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B42" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>227</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>12</v>
@@ -3128,36 +3149,36 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="J42" s="10" t="s">
-        <v>229</v>
+        <v>225</v>
+      </c>
+      <c r="J42" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="L42" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>22</v>
+      <c r="B43" s="6" t="s">
+        <v>231</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D43" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>231</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>12</v>
@@ -3166,16 +3187,54 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="J43" s="6" t="s">
         <v>235</v>
       </c>
+      <c r="J43" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="K43" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="30" customHeight="1">
+      <c r="A44" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L44" s="10" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3190,7 +3249,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -3212,7 +3271,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3220,13 +3279,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3234,13 +3293,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3249,38 +3308,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G44)</f>
+        <f>SUM(G10:G45)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3300,16 +3359,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3422,22 +3481,22 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1">
+    <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
         <v>55</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>59</v>
-      </c>
       <c r="E15" s="19">
-        <f>CEILING(BoardQty*10,1)</f>
-        <v>10</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G15" s="20">
         <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
@@ -3446,38 +3505,38 @@
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1">
       <c r="A16" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>67</v>
-      </c>
       <c r="E16" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*10,1)</f>
+        <v>10</v>
       </c>
       <c r="G16" s="20">
         <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1">
+    <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -3490,10 +3549,10 @@
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1">
       <c r="A18" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>80</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>79</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>81</v>
@@ -3510,44 +3569,44 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>86</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>89</v>
-      </c>
       <c r="E19" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1">
+    <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="C20" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>97</v>
-      </c>
       <c r="E20" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
@@ -3556,16 +3615,16 @@
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="C21" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>104</v>
       </c>
       <c r="E21" s="19">
         <f>BoardQty*1</f>
@@ -3576,22 +3635,22 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>112</v>
-      </c>
       <c r="E22" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G22" s="20">
         <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
@@ -3600,16 +3659,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3620,22 +3679,22 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1">
+    <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>128</v>
-      </c>
       <c r="E24" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G24" s="20">
         <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
@@ -3644,16 +3703,16 @@
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>135</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>136</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -3664,18 +3723,18 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -3686,12 +3745,12 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>147</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>146</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>148</v>
@@ -3713,13 +3772,13 @@
         <v>154</v>
       </c>
       <c r="B28" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>156</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>157</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -3732,42 +3791,42 @@
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>165</v>
-      </c>
       <c r="E29" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G29" s="20">
         <f>IF(AND(ISNUMBER(E29),ISNUMBER(F29)),E29*F29,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
         <v>169</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E30" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
@@ -3779,7 +3838,7 @@
         <v>176</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>58</v>
+        <v>175</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>177</v>
@@ -3798,16 +3857,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="19" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>182</v>
+        <v>65</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E32" s="19">
         <f>BoardQty*1</f>
@@ -3820,16 +3879,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>178</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -3842,42 +3901,42 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E34" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G34" s="20">
         <f>IF(AND(ISNUMBER(E34),ISNUMBER(F34)),E34*F34,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" customHeight="1">
+    <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="E35" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G35" s="20">
         <f>IF(AND(ISNUMBER(E35),ISNUMBER(F35)),E35*F35,"")</f>
@@ -3886,16 +3945,16 @@
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -3908,16 +3967,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>197</v>
-      </c>
       <c r="D37" s="19" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -3930,16 +3989,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -3952,16 +4011,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -3974,16 +4033,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -3996,16 +4055,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4018,16 +4077,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4040,16 +4099,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B43" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>225</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>228</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4062,16 +4121,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>231</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4082,17 +4141,39 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>262</v>
+    <row r="45" spans="1:7" ht="30" customHeight="1">
+      <c r="A45" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E45" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G45" s="20">
+        <f>IF(AND(ISNUMBER(E45),ISNUMBER(F45)),E45*F45,"")</f>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="23" t="s">
-        <v>263</v>
+      <c r="A48" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="23" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -4275,6 +4356,11 @@
       <formula>AND(ISBLANK(D44),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="expression" dxfId="0" priority="36">
+      <formula>AND(ISBLANK(D45),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -4311,10 +4397,11 @@
     <hyperlink ref="D42" r:id="rId33"/>
     <hyperlink ref="D43" r:id="rId34"/>
     <hyperlink ref="D44" r:id="rId35"/>
+    <hyperlink ref="D45" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId36"/>
-  <legacyDrawing r:id="rId37"/>
+  <drawing r:id="rId37"/>
+  <legacyDrawing r:id="rId38"/>
 </worksheet>
 </file>
 
@@ -4331,72 +4418,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@21c7d4732b43b4d3e347ca5fe547c2fa612cb327 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -340,10 +340,10 @@
     <t>10</t>
   </si>
   <si>
-    <t>https://cdn.sparkfun.com/datasheets/Components/LED/COM-12877.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/sparkfun-electronics/COM-12986/5673799</t>
+    <t>https://cdn.sparkfun.com/assets/6/9/0/f/3/DS-12999-LED_-_RGB_Addressable__PTH__5mm_Clear__5_Pack_.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/sparkfun-electronics/COM-12999/5673800</t>
   </si>
   <si>
     <t>8</t>
@@ -949,7 +949,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-07 09:51:47</t>
+    <t>2023-04-07 10:55:49</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@82edcbd28179428aa499f036150e6cd5850752b6 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="292">
   <si>
     <t>Row</t>
   </si>
@@ -322,6 +322,27 @@
     <t>7</t>
   </si>
   <si>
+    <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
+  </si>
+  <si>
+    <t>1N5817</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D_DO-41_SOD81_P10.16mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/1n5817-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/onsemi/1N5817RLG/807254</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>RGB LED with integrated controller, 5mm/8mm LED package</t>
   </si>
   <si>
@@ -346,7 +367,7 @@
     <t>https://www.digikey.ch/de/products/detail/sparkfun-electronics/COM-12999/5673800</t>
   </si>
   <si>
-    <t>8</t>
+    <t>9</t>
   </si>
   <si>
     <t>Resettable fuse, polymeric positive temperature coefficient</t>
@@ -370,9 +391,6 @@
     <t>https://www.digikey.ch/de/products/detail/bel-fuse-inc/0ZRP0090FF1E/9468255</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>DC Barrel Jack with an internal switch</t>
   </si>
   <si>
@@ -394,6 +412,9 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -412,9 +433,6 @@
     <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
   </si>
   <si>
@@ -436,6 +454,9 @@
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>expansion header for Raspberry Pi 2 &amp; 3</t>
   </si>
   <si>
@@ -457,7 +478,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -481,7 +502,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
@@ -505,7 +526,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
@@ -529,7 +550,7 @@
     <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x02, script generated</t>
@@ -553,7 +574,7 @@
     <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x03, script generated</t>
@@ -577,7 +598,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>J7</t>
@@ -595,7 +616,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>USB Type A connector</t>
@@ -616,7 +637,7 @@
     <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>Inductor</t>
@@ -640,7 +661,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/7447471022/2794428</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>Inductor with ferrite core</t>
@@ -664,7 +685,7 @@
     <t>https://www.digikey.ch/en/products/detail/fair-rite-products-corp/2743005111/8599429</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>PDQE15-Q24-S5-D</t>
@@ -682,7 +703,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -703,7 +724,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C100J/13537327</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>R3</t>
@@ -715,7 +736,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C330J/13537493</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>R1</t>
@@ -727,7 +748,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C221J/13537314</t>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>R2 R5</t>
@@ -739,7 +760,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C471J/13537235</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -763,7 +784,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430466043726/5209037</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>SW5</t>
@@ -772,19 +793,19 @@
     <t>B</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>SW6</t>
   </si>
   <si>
-    <t>30</t>
+    <t>31</t>
   </si>
   <si>
     <t>SW1</t>
   </si>
   <si>
-    <t>31</t>
+    <t>32</t>
   </si>
   <si>
     <t>SW2</t>
@@ -793,15 +814,15 @@
     <t>E</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>SW3</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
   </si>
   <si>
@@ -823,7 +844,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
   </si>
   <si>
-    <t>34</t>
+    <t>35</t>
   </si>
   <si>
     <t>SW7</t>
@@ -832,7 +853,7 @@
     <t>VOL Rotary</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
@@ -853,7 +874,7 @@
     <t>https://www.digikey.ch/de/products/detail/onsemi/H11L1M/284866</t>
   </si>
   <si>
-    <t>36</t>
+    <t>37</t>
   </si>
   <si>
     <t>Pico</t>
@@ -910,7 +931,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>71 (0 SMD/ 69 THT)</t>
+    <t>72 (0 SMD/ 70 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -949,7 +970,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-07 10:55:49</t>
+    <t>2023-04-07 12:34:16</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
@@ -1724,7 +1745,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1749,7 +1770,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1763,55 +1784,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="F2" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1819,16 +1840,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="F6" s="3">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2111,19 +2132,19 @@
         <v>62</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="G15" s="5" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>21</v>
@@ -2132,65 +2153,65 @@
         <v>21</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="G16" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I16" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>12</v>
@@ -2199,33 +2220,33 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="6" t="s">
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="60" customHeight="1">
-      <c r="A18" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="C18" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>85</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>87</v>
@@ -2249,7 +2270,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="30" customHeight="1">
+    <row r="19" spans="1:12" ht="60" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>90</v>
       </c>
@@ -2263,28 +2284,28 @@
         <v>93</v>
       </c>
       <c r="E19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="G19" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I19" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
@@ -2292,57 +2313,57 @@
         <v>26</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>102</v>
-      </c>
       <c r="G20" s="9" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="10" t="s">
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="60" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>12</v>
@@ -2351,74 +2372,74 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="6" t="s">
+    </row>
+    <row r="22" spans="1:12" ht="60" customHeight="1">
+      <c r="A22" s="9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="30" customHeight="1">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="G22" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="10" t="s">
         <v>119</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>126</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>18</v>
@@ -2427,74 +2448,74 @@
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>134</v>
-      </c>
       <c r="G24" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L24" s="10" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>12</v>
@@ -2503,36 +2524,36 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="C26" s="11" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>12</v>
@@ -2541,7 +2562,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>21</v>
@@ -2550,24 +2571,24 @@
         <v>21</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>155</v>
@@ -2605,10 +2626,10 @@
         <v>161</v>
       </c>
       <c r="E28" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>12</v>
@@ -2617,62 +2638,62 @@
         <v>19</v>
       </c>
       <c r="I28" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="10" t="s">
         <v>164</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" s="10" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>174</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>175</v>
@@ -2681,19 +2702,19 @@
         <v>176</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>21</v>
@@ -2702,15 +2723,15 @@
         <v>21</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B31" s="6" t="s">
         <v>181</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>182</v>
@@ -2719,7 +2740,7 @@
         <v>183</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>65</v>
+        <v>182</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>184</v>
@@ -2748,19 +2769,19 @@
         <v>187</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>189</v>
+        <v>72</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>12</v>
@@ -2769,7 +2790,7 @@
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="J32" s="12" t="s">
         <v>21</v>
@@ -2778,27 +2799,27 @@
         <v>21</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>12</v>
@@ -2807,7 +2828,7 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>21</v>
@@ -2816,36 +2837,36 @@
         <v>21</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>21</v>
@@ -2854,65 +2875,65 @@
         <v>21</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>200</v>
-      </c>
       <c r="C36" s="11" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>12</v>
@@ -2921,7 +2942,7 @@
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>21</v>
@@ -2930,27 +2951,27 @@
         <v>21</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D37" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
@@ -2959,7 +2980,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>21</v>
@@ -2968,27 +2989,27 @@
         <v>21</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -2997,7 +3018,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>21</v>
@@ -3006,27 +3027,27 @@
         <v>21</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>216</v>
+        <v>49</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -3035,7 +3056,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J39" s="8" t="s">
         <v>21</v>
@@ -3044,27 +3065,27 @@
         <v>21</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3073,7 +3094,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>21</v>
@@ -3082,27 +3103,27 @@
         <v>21</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3111,7 +3132,7 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>21</v>
@@ -3120,27 +3141,27 @@
         <v>21</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>220</v>
-      </c>
       <c r="C42" s="11" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>12</v>
@@ -3149,7 +3170,7 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>21</v>
@@ -3158,27 +3179,27 @@
         <v>21</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>12</v>
@@ -3187,7 +3208,7 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>21</v>
@@ -3196,27 +3217,27 @@
         <v>21</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>21</v>
+      <c r="B44" s="10" t="s">
+        <v>238</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D44" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="E44" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>238</v>
-      </c>
       <c r="F44" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>12</v>
@@ -3225,7 +3246,7 @@
         <v>19</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>21</v>
@@ -3234,7 +3255,45 @@
         <v>21</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="30" customHeight="1">
+      <c r="A45" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -3249,7 +3308,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -3271,7 +3330,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3279,13 +3338,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3293,13 +3352,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3308,38 +3367,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G45)</f>
+        <f>SUM(G10:G46)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3359,16 +3418,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3503,62 +3562,62 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1">
+    <row r="16" spans="1:7">
       <c r="A16" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B16" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="D16" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>66</v>
-      </c>
       <c r="E16" s="19">
-        <f>CEILING(BoardQty*10,1)</f>
-        <v>10</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G16" s="20">
         <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>74</v>
-      </c>
       <c r="E17" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*10,1)</f>
+        <v>10</v>
       </c>
       <c r="G17" s="20">
         <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1">
+    <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>81</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>82</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -3571,10 +3630,10 @@
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>86</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>85</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>87</v>
@@ -3591,44 +3650,44 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
         <v>93</v>
       </c>
       <c r="B20" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="D20" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>96</v>
-      </c>
       <c r="E20" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1">
+    <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="C21" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>103</v>
-      </c>
       <c r="E21" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
@@ -3637,16 +3696,16 @@
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>110</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>111</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -3657,22 +3716,22 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>119</v>
-      </c>
       <c r="E23" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -3681,16 +3740,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>127</v>
       </c>
       <c r="E24" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3701,22 +3760,22 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" customHeight="1">
+    <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>135</v>
-      </c>
       <c r="E25" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G25" s="20">
         <f>IF(AND(ISNUMBER(E25),ISNUMBER(F25)),E25*F25,"")</f>
@@ -3725,16 +3784,16 @@
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1">
       <c r="A26" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>142</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>143</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -3745,18 +3804,18 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -3767,12 +3826,12 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1">
+    <row r="28" spans="1:7">
       <c r="A28" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>153</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>155</v>
@@ -3794,13 +3853,13 @@
         <v>161</v>
       </c>
       <c r="B29" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>163</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>164</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -3813,42 +3872,42 @@
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>172</v>
-      </c>
       <c r="E30" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G30" s="20">
         <f>IF(AND(ISNUMBER(E30),ISNUMBER(F30)),E30*F30,"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
         <v>176</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E31" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
@@ -3860,7 +3919,7 @@
         <v>183</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>65</v>
+        <v>182</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>184</v>
@@ -3879,16 +3938,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>189</v>
+        <v>72</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -3901,16 +3960,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>192</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>185</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -3923,42 +3982,42 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E35" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G35" s="20">
         <f>IF(AND(ISNUMBER(E35),ISNUMBER(F35)),E35*F35,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="30" customHeight="1">
+    <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E36" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G36" s="20">
         <f>IF(AND(ISNUMBER(E36),ISNUMBER(F36)),E36*F36,"")</f>
@@ -3967,16 +4026,16 @@
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
       <c r="A37" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E37" s="19">
         <f>BoardQty*1</f>
@@ -3989,16 +4048,16 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
       <c r="A38" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>204</v>
-      </c>
       <c r="D38" s="19" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -4011,16 +4070,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -4033,16 +4092,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>216</v>
+        <v>49</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -4055,16 +4114,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4077,16 +4136,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4099,16 +4158,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4121,16 +4180,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B44" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>232</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>234</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>235</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4143,16 +4202,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>238</v>
-      </c>
       <c r="C45" s="19" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -4163,17 +4222,39 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="23" t="s">
-        <v>270</v>
+    <row r="46" spans="1:7" ht="30" customHeight="1">
+      <c r="A46" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="E46" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G46" s="20">
+        <f>IF(AND(ISNUMBER(E46),ISNUMBER(F46)),E46*F46,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="23" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -4361,6 +4442,11 @@
       <formula>AND(ISBLANK(D45),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule type="expression" dxfId="0" priority="37">
+      <formula>AND(ISBLANK(D46),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -4398,10 +4484,11 @@
     <hyperlink ref="D43" r:id="rId34"/>
     <hyperlink ref="D44" r:id="rId35"/>
     <hyperlink ref="D45" r:id="rId36"/>
+    <hyperlink ref="D46" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId37"/>
-  <legacyDrawing r:id="rId38"/>
+  <drawing r:id="rId38"/>
+  <legacyDrawing r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -4418,72 +4505,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@da33b3c386730a44478dbe078ebce51a83107912 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -910,7 +910,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>1.0.2</t>
+    <t>2.0.0-RC1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -970,7 +970,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-07 14:23:56</t>
+    <t>2023-04-15 09:43:55</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.6.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@a9c49d1700ae429b07668568396d295bc0803791 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -970,10 +970,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-15 23:00:18</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
+    <t>2023-04-16 11:03:22</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.16 + KiBot v1.6.1</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@7a98c0943bab17faa8a58335fede2286062115ea 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="298">
   <si>
     <t>Row</t>
   </si>
@@ -391,6 +391,24 @@
     <t>https://www.digikey.ch/de/products/detail/bel-fuse-inc/0ZRP0090FF1E/9468255</t>
   </si>
   <si>
+    <t>Fuse, small symbol</t>
+  </si>
+  <si>
+    <t>Fuse_Small</t>
+  </si>
+  <si>
+    <t>F2 F3</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Trace_Fuse</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>DC Barrel Jack with an internal switch</t>
   </si>
   <si>
@@ -412,9 +430,6 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -433,6 +448,9 @@
     <t>https://www.digikey.ch/de/products/detail/amphenol-cs-fci/68016-202HLF/4273561</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
   </si>
   <si>
@@ -454,7 +472,7 @@
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>expansion header for Raspberry Pi 2 &amp; 3</t>
@@ -478,7 +496,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -502,7 +520,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
@@ -526,7 +544,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
@@ -550,7 +568,7 @@
     <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x02, script generated</t>
@@ -574,7 +592,7 @@
     <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x03, script generated</t>
@@ -598,7 +616,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>J7</t>
@@ -616,7 +634,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>USB Type A connector</t>
@@ -637,7 +655,7 @@
     <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>Inductor</t>
@@ -661,7 +679,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/7447471022/2794428</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>Inductor with ferrite core</t>
@@ -685,7 +703,7 @@
     <t>https://www.digikey.ch/en/products/detail/fair-rite-products-corp/2743005111/8599429</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>PDQE15-Q24-S5-D</t>
@@ -703,7 +721,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -724,7 +742,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C100J/13537327</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>R3</t>
@@ -736,7 +754,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C330J/13537493</t>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>R1</t>
@@ -748,7 +766,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C221J/13537314</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>R2 R5</t>
@@ -760,7 +778,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C471J/13537235</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -784,7 +802,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430466043726/5209037</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>SW5</t>
@@ -793,34 +811,34 @@
     <t>B</t>
   </si>
   <si>
-    <t>30</t>
+    <t>31</t>
   </si>
   <si>
     <t>SW6</t>
   </si>
   <si>
-    <t>31</t>
+    <t>32</t>
   </si>
   <si>
     <t>SW1</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>SW2</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>SW3</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>34</t>
+    <t>35</t>
   </si>
   <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
@@ -844,7 +862,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>SW7</t>
@@ -853,7 +871,7 @@
     <t>VOL Rotary</t>
   </si>
   <si>
-    <t>36</t>
+    <t>37</t>
   </si>
   <si>
     <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
@@ -874,7 +892,7 @@
     <t>https://www.digikey.ch/de/products/detail/onsemi/H11L1M/284866</t>
   </si>
   <si>
-    <t>37</t>
+    <t>38</t>
   </si>
   <si>
     <t>Pico</t>
@@ -931,7 +949,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>72 (0 SMD/ 70 THT)</t>
+    <t>74 (2 SMD/ 70 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -970,7 +988,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-16 11:03:22</t>
+    <t>2023-04-16 12:28:04</t>
   </si>
   <si>
     <t>KiCost® v1.1.16 + KiBot v1.6.1</t>
@@ -1745,7 +1763,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1770,7 +1788,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1784,55 +1802,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="F2" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1840,16 +1858,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="F6" s="3">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2232,7 +2250,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
+    <row r="18" spans="1:12">
       <c r="A18" s="9" t="s">
         <v>72</v>
       </c>
@@ -2245,49 +2263,49 @@
       <c r="D18" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="12" t="s">
         <v>86</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>87</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="10" t="s">
+      <c r="B19" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="60" customHeight="1">
-      <c r="A19" s="5" t="s">
+      <c r="C19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>92</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>12</v>
@@ -2296,45 +2314,45 @@
         <v>19</v>
       </c>
       <c r="I19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" customHeight="1">
+    </row>
+    <row r="20" spans="1:12" ht="60" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>101</v>
-      </c>
       <c r="G20" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J20" s="12" t="s">
         <v>21</v>
@@ -2343,65 +2361,65 @@
         <v>21</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="G21" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" customHeight="1">
+      <c r="A22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="6" t="s">
+      <c r="B22" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="60" customHeight="1">
-      <c r="A22" s="9" t="s">
+      <c r="C22" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="D22" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>12</v>
@@ -2410,45 +2428,45 @@
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="60" customHeight="1">
+      <c r="A23" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J22" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L22" s="10" t="s">
+      <c r="B23" s="6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="5" t="s">
+      <c r="C23" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="G23" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>21</v>
@@ -2457,27 +2475,27 @@
         <v>21</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="D24" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>133</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>18</v>
@@ -2486,7 +2504,7 @@
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>21</v>
@@ -2495,36 +2513,36 @@
         <v>21</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>141</v>
-      </c>
       <c r="G25" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>21</v>
@@ -2533,27 +2551,27 @@
         <v>21</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="D26" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>149</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>12</v>
@@ -2562,7 +2580,7 @@
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>21</v>
@@ -2571,18 +2589,18 @@
         <v>21</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>153</v>
@@ -2617,19 +2635,19 @@
         <v>158</v>
       </c>
       <c r="B28" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>161</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>160</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>12</v>
@@ -2638,36 +2656,36 @@
         <v>19</v>
       </c>
       <c r="I28" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="10" t="s">
         <v>163</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" s="10" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
@@ -2676,7 +2694,7 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>21</v>
@@ -2685,36 +2703,36 @@
         <v>21</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="D30" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>178</v>
-      </c>
       <c r="G30" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>21</v>
@@ -2723,30 +2741,30 @@
         <v>21</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>184</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>19</v>
@@ -2768,20 +2786,20 @@
       <c r="A32" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="D32" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="E32" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>190</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>191</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>12</v>
@@ -2790,36 +2808,36 @@
         <v>19</v>
       </c>
       <c r="I32" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>188</v>
-      </c>
       <c r="C33" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>196</v>
+        <v>72</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>12</v>
@@ -2828,7 +2846,7 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>21</v>
@@ -2837,27 +2855,27 @@
         <v>21</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>12</v>
@@ -2866,7 +2884,7 @@
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>21</v>
@@ -2875,36 +2893,36 @@
         <v>21</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>21</v>
@@ -2913,18 +2931,18 @@
         <v>21</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>209</v>
@@ -2933,16 +2951,16 @@
         <v>210</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>21</v>
@@ -2951,18 +2969,18 @@
         <v>21</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>214</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>215</v>
@@ -2971,7 +2989,7 @@
         <v>216</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>12</v>
@@ -2980,7 +2998,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>21</v>
@@ -2989,27 +3007,27 @@
         <v>21</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" s="11" t="s">
         <v>217</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -3018,7 +3036,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>21</v>
@@ -3027,27 +3045,27 @@
         <v>21</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -3056,7 +3074,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="J39" s="8" t="s">
         <v>21</v>
@@ -3065,27 +3083,27 @@
         <v>21</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>223</v>
+        <v>49</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3094,7 +3112,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>21</v>
@@ -3103,27 +3121,27 @@
         <v>21</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3132,7 +3150,7 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>21</v>
@@ -3141,27 +3159,27 @@
         <v>21</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>12</v>
@@ -3170,7 +3188,7 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>21</v>
@@ -3179,18 +3197,18 @@
         <v>21</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>228</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>235</v>
@@ -3199,7 +3217,7 @@
         <v>236</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>12</v>
@@ -3208,7 +3226,7 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>21</v>
@@ -3217,27 +3235,27 @@
         <v>21</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>237</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>241</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>12</v>
@@ -3246,7 +3264,7 @@
         <v>19</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>21</v>
@@ -3255,15 +3273,15 @@
         <v>21</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>245</v>
@@ -3294,6 +3312,44 @@
       </c>
       <c r="L45" s="6" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="30" customHeight="1">
+      <c r="A46" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L46" s="10" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3308,7 +3364,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -3330,7 +3386,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3338,13 +3394,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3352,13 +3408,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3367,38 +3423,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G46)</f>
+        <f>SUM(G10:G47)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3418,16 +3474,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3628,7 +3684,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1">
+    <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
         <v>85</v>
       </c>
@@ -3638,12 +3694,9 @@
       <c r="C19" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>88</v>
-      </c>
       <c r="E19" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
@@ -3652,16 +3705,16 @@
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>92</v>
       </c>
       <c r="C20" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>94</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>95</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -3672,44 +3725,44 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="D21" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>102</v>
-      </c>
       <c r="E21" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1">
+    <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>110</v>
-      </c>
       <c r="E22" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G22" s="20">
         <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
@@ -3718,16 +3771,16 @@
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="D23" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>118</v>
       </c>
       <c r="E23" s="19">
         <f>BoardQty*1</f>
@@ -3738,22 +3791,22 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>126</v>
-      </c>
       <c r="E24" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G24" s="20">
         <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
@@ -3762,16 +3815,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>132</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>134</v>
       </c>
       <c r="E25" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3782,22 +3835,22 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>142</v>
-      </c>
       <c r="E26" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G26" s="20">
         <f>IF(AND(ISNUMBER(E26),ISNUMBER(F26)),E26*F26,"")</f>
@@ -3806,16 +3859,16 @@
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="D27" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>150</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -3826,7 +3879,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
         <v>153</v>
       </c>
@@ -3848,18 +3901,18 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>160</v>
       </c>
       <c r="C29" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" s="19" t="s">
         <v>162</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>163</v>
       </c>
       <c r="E29" s="19">
         <f>BoardQty*1</f>
@@ -3872,16 +3925,16 @@
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1">
       <c r="A30" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="D30" s="19" t="s">
         <v>169</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>171</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -3894,32 +3947,32 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>179</v>
-      </c>
       <c r="E31" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G31" s="20">
         <f>IF(AND(ISNUMBER(E31),ISNUMBER(F31)),E31*F31,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>183</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>182</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>184</v>
@@ -3928,8 +3981,8 @@
         <v>185</v>
       </c>
       <c r="E32" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G32" s="20">
         <f>IF(AND(ISNUMBER(E32),ISNUMBER(F32)),E32*F32,"")</f>
@@ -3938,16 +3991,16 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="19" t="s">
+      <c r="D33" s="19" t="s">
         <v>191</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>192</v>
       </c>
       <c r="E33" s="19">
         <f>BoardQty*1</f>
@@ -3960,16 +4013,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>196</v>
+        <v>72</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -3982,16 +4035,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -4004,27 +4057,27 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E36" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G36" s="20">
         <f>IF(AND(ISNUMBER(E36),ISNUMBER(F36)),E36*F36,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30" customHeight="1">
+    <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
         <v>209</v>
       </c>
@@ -4032,14 +4085,14 @@
         <v>210</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="E37" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G37" s="20">
         <f>IF(AND(ISNUMBER(E37),ISNUMBER(F37)),E37*F37,"")</f>
@@ -4054,10 +4107,10 @@
         <v>216</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E38" s="19">
         <f>BoardQty*1</f>
@@ -4070,16 +4123,16 @@
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
       <c r="A39" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="19" t="s">
         <v>218</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>212</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -4092,16 +4145,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -4114,16 +4167,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>223</v>
+        <v>49</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4136,16 +4189,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4158,16 +4211,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4186,10 +4239,10 @@
         <v>236</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4202,16 +4255,16 @@
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -4244,17 +4297,39 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="21" t="s">
-        <v>275</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>276</v>
+    <row r="47" spans="1:7" ht="30" customHeight="1">
+      <c r="A47" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="E47" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G47" s="20">
+        <f>IF(AND(ISNUMBER(E47),ISNUMBER(F47)),E47*F47,"")</f>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="23" t="s">
-        <v>277</v>
+      <c r="A50" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="23" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -4447,6 +4522,11 @@
       <formula>AND(ISBLANK(D46),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="expression" dxfId="0" priority="38">
+      <formula>AND(ISBLANK(D47),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -4457,34 +4537,34 @@
     <hyperlink ref="D16" r:id="rId7"/>
     <hyperlink ref="D17" r:id="rId8"/>
     <hyperlink ref="D18" r:id="rId9"/>
-    <hyperlink ref="D19" r:id="rId10"/>
-    <hyperlink ref="D20" r:id="rId11"/>
-    <hyperlink ref="D21" r:id="rId12"/>
-    <hyperlink ref="D22" r:id="rId13"/>
-    <hyperlink ref="D23" r:id="rId14"/>
-    <hyperlink ref="D24" r:id="rId15"/>
-    <hyperlink ref="D25" r:id="rId16"/>
-    <hyperlink ref="D26" r:id="rId17"/>
-    <hyperlink ref="D27" r:id="rId18"/>
-    <hyperlink ref="D28" r:id="rId19"/>
-    <hyperlink ref="D29" r:id="rId20"/>
-    <hyperlink ref="D30" r:id="rId21"/>
-    <hyperlink ref="D31" r:id="rId22"/>
-    <hyperlink ref="D32" r:id="rId23"/>
-    <hyperlink ref="D33" r:id="rId24"/>
-    <hyperlink ref="D34" r:id="rId25"/>
-    <hyperlink ref="D35" r:id="rId26"/>
-    <hyperlink ref="D36" r:id="rId27"/>
-    <hyperlink ref="D37" r:id="rId28"/>
-    <hyperlink ref="D38" r:id="rId29"/>
-    <hyperlink ref="D39" r:id="rId30"/>
-    <hyperlink ref="D40" r:id="rId31"/>
-    <hyperlink ref="D41" r:id="rId32"/>
-    <hyperlink ref="D42" r:id="rId33"/>
-    <hyperlink ref="D43" r:id="rId34"/>
-    <hyperlink ref="D44" r:id="rId35"/>
-    <hyperlink ref="D45" r:id="rId36"/>
-    <hyperlink ref="D46" r:id="rId37"/>
+    <hyperlink ref="D20" r:id="rId10"/>
+    <hyperlink ref="D21" r:id="rId11"/>
+    <hyperlink ref="D22" r:id="rId12"/>
+    <hyperlink ref="D23" r:id="rId13"/>
+    <hyperlink ref="D24" r:id="rId14"/>
+    <hyperlink ref="D25" r:id="rId15"/>
+    <hyperlink ref="D26" r:id="rId16"/>
+    <hyperlink ref="D27" r:id="rId17"/>
+    <hyperlink ref="D28" r:id="rId18"/>
+    <hyperlink ref="D29" r:id="rId19"/>
+    <hyperlink ref="D30" r:id="rId20"/>
+    <hyperlink ref="D31" r:id="rId21"/>
+    <hyperlink ref="D32" r:id="rId22"/>
+    <hyperlink ref="D33" r:id="rId23"/>
+    <hyperlink ref="D34" r:id="rId24"/>
+    <hyperlink ref="D35" r:id="rId25"/>
+    <hyperlink ref="D36" r:id="rId26"/>
+    <hyperlink ref="D37" r:id="rId27"/>
+    <hyperlink ref="D38" r:id="rId28"/>
+    <hyperlink ref="D39" r:id="rId29"/>
+    <hyperlink ref="D40" r:id="rId30"/>
+    <hyperlink ref="D41" r:id="rId31"/>
+    <hyperlink ref="D42" r:id="rId32"/>
+    <hyperlink ref="D43" r:id="rId33"/>
+    <hyperlink ref="D44" r:id="rId34"/>
+    <hyperlink ref="D45" r:id="rId35"/>
+    <hyperlink ref="D46" r:id="rId36"/>
+    <hyperlink ref="D47" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId38"/>
@@ -4505,72 +4585,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@72db4be23bc253df286be30be735b9595d2a3f78 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -397,7 +397,7 @@
     <t>Fuse_Small</t>
   </si>
   <si>
-    <t>F2 F3</t>
+    <t>F2 F3 F4 F5</t>
   </si>
   <si>
     <t>~</t>
@@ -949,7 +949,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>74 (2 SMD/ 70 THT)</t>
+    <t>76 (4 SMD/ 70 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -988,7 +988,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-16 12:28:04</t>
+    <t>2023-04-16 12:41:36</t>
   </si>
   <si>
     <t>KiCost® v1.1.16 + KiBot v1.6.1</t>
@@ -1867,7 +1867,7 @@
         <v>272</v>
       </c>
       <c r="F6" s="3">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2270,7 +2270,7 @@
         <v>87</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>19</v>
@@ -3695,8 +3695,8 @@
         <v>87</v>
       </c>
       <c r="E19" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@7de85133f31992207a04b2058f6d343e71cb437c 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -928,7 +928,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>2.0.0-RC1</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Date:</t>
@@ -988,7 +988,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-04-16 12:41:36</t>
+    <t>2023-04-24 18:46:53</t>
   </si>
   <si>
     <t>KiCost® v1.1.16 + KiBot v1.6.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@20cddacd12251397b1db9bb04de7b150b56f5559 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -928,7 +928,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>2.1.0-RC1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -940,7 +940,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.1.1-36-gbcf78dbe24-dirty-deb11</t>
+    <t>7.0.5.1-1-g8f565ef7f0-dirty-deb11</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -988,10 +988,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-05-13 09:00:49</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.16 + KiBot v1.6.1</t>
+    <t>2023-06-05 17:22:28</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -3379,7 +3379,7 @@
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@d4cd88aa4ff3c0901df7fe97760083c110936a46 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="304">
   <si>
     <t>Row</t>
   </si>
@@ -499,6 +499,24 @@
     <t>15</t>
   </si>
   <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J18 J19 J20 J21 J22 J23</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>PinHeader_2x02_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -520,7 +538,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300621021/4846834</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
@@ -544,7 +562,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
@@ -568,7 +586,7 @@
     <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x02, script generated</t>
@@ -592,7 +610,7 @@
     <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
   </si>
   <si>
-    <t>19</t>
+    <t>20</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x03, script generated</t>
@@ -616,7 +634,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
   </si>
   <si>
-    <t>20</t>
+    <t>21</t>
   </si>
   <si>
     <t>J7</t>
@@ -634,7 +652,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021121/4846886</t>
   </si>
   <si>
-    <t>21</t>
+    <t>22</t>
   </si>
   <si>
     <t>USB Type A connector</t>
@@ -655,7 +673,7 @@
     <t>https://www.digikey.ch/de/products/detail/gct/USB1061-GF-L-A/10649776</t>
   </si>
   <si>
-    <t>22</t>
+    <t>23</t>
   </si>
   <si>
     <t>Inductor</t>
@@ -679,7 +697,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/7447471022/2794428</t>
   </si>
   <si>
-    <t>23</t>
+    <t>24</t>
   </si>
   <si>
     <t>Inductor with ferrite core</t>
@@ -703,7 +721,7 @@
     <t>https://www.digikey.ch/en/products/detail/fair-rite-products-corp/2743005111/8599429</t>
   </si>
   <si>
-    <t>24</t>
+    <t>25</t>
   </si>
   <si>
     <t>PDQE15-Q24-S5-D</t>
@@ -721,7 +739,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-inc/PDQE15-Q24-S5-D/10230147</t>
   </si>
   <si>
-    <t>25</t>
+    <t>26</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -742,7 +760,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C100J/13537327</t>
   </si>
   <si>
-    <t>26</t>
+    <t>27</t>
   </si>
   <si>
     <t>R3</t>
@@ -754,7 +772,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C330J/13537493</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>R1</t>
@@ -766,7 +784,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C221J/13537314</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>R2 R5</t>
@@ -778,7 +796,7 @@
     <t>https://www.digikey.ch/de/products/detail/koa-speer-electronics-inc/CF1-4C471J/13537235</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
@@ -802,7 +820,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430466043726/5209037</t>
   </si>
   <si>
-    <t>30</t>
+    <t>31</t>
   </si>
   <si>
     <t>SW5</t>
@@ -811,25 +829,25 @@
     <t>B</t>
   </si>
   <si>
-    <t>31</t>
+    <t>32</t>
   </si>
   <si>
     <t>SW6</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>SW1</t>
   </si>
   <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>SW2</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>34</t>
+    <t>35</t>
   </si>
   <si>
     <t>SW3</t>
@@ -838,7 +856,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
@@ -862,7 +880,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
   </si>
   <si>
-    <t>36</t>
+    <t>37</t>
   </si>
   <si>
     <t>SW7</t>
@@ -871,7 +889,7 @@
     <t>VOL Rotary</t>
   </si>
   <si>
-    <t>37</t>
+    <t>38</t>
   </si>
   <si>
     <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
@@ -892,7 +910,7 @@
     <t>https://www.digikey.ch/de/products/detail/onsemi/H11L1M/284866</t>
   </si>
   <si>
-    <t>38</t>
+    <t>39</t>
   </si>
   <si>
     <t>Pico</t>
@@ -949,7 +967,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>76 (4 SMD/ 70 THT)</t>
+    <t>82 (4 SMD/ 76 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -988,7 +1006,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-05 17:48:50</t>
+    <t>2023-06-09 15:09:11</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -1763,7 +1781,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1788,7 +1806,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1802,55 +1820,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="F2" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1858,16 +1876,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="F6" s="3">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2440,7 +2458,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="60" customHeight="1">
+    <row r="23" spans="1:12" ht="45" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>118</v>
       </c>
@@ -2460,51 +2478,51 @@
         <v>123</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="60" customHeight="1">
+      <c r="A24" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="6" t="s">
+      <c r="B24" s="10" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1">
-      <c r="A24" s="9" t="s">
+      <c r="C24" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="D24" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>131</v>
-      </c>
       <c r="G24" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>21</v>
@@ -2513,27 +2531,27 @@
         <v>21</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>139</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>18</v>
@@ -2542,7 +2560,7 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>21</v>
@@ -2551,36 +2569,36 @@
         <v>21</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="D26" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>147</v>
-      </c>
       <c r="G26" s="9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>21</v>
@@ -2589,27 +2607,27 @@
         <v>21</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="D27" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>155</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>12</v>
@@ -2618,7 +2636,7 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>21</v>
@@ -2627,18 +2645,18 @@
         <v>21</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>159</v>
@@ -2673,19 +2691,19 @@
         <v>164</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>166</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>12</v>
@@ -2694,36 +2712,36 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="E30" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>174</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>176</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>12</v>
@@ -2732,7 +2750,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>21</v>
@@ -2741,36 +2759,36 @@
         <v>21</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="D31" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="G31" s="5" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>21</v>
@@ -2779,30 +2797,30 @@
         <v>21</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="11" t="s">
+      <c r="D32" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="E32" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>190</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>19</v>
@@ -2824,20 +2842,20 @@
       <c r="A33" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>12</v>
@@ -2846,36 +2864,36 @@
         <v>19</v>
       </c>
       <c r="I33" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>194</v>
-      </c>
       <c r="C34" s="11" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>202</v>
+        <v>72</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>12</v>
@@ -2884,7 +2902,7 @@
         <v>19</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>21</v>
@@ -2893,27 +2911,27 @@
         <v>21</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>12</v>
@@ -2922,7 +2940,7 @@
         <v>19</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>21</v>
@@ -2931,36 +2949,36 @@
         <v>21</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>21</v>
@@ -2969,18 +2987,18 @@
         <v>21</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>215</v>
@@ -2989,16 +3007,16 @@
         <v>216</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>21</v>
@@ -3007,18 +3025,18 @@
         <v>21</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1">
       <c r="A38" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>220</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>214</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>221</v>
@@ -3027,7 +3045,7 @@
         <v>222</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>12</v>
@@ -3036,7 +3054,7 @@
         <v>19</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>21</v>
@@ -3045,27 +3063,27 @@
         <v>21</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>12</v>
@@ -3074,7 +3092,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="J39" s="8" t="s">
         <v>21</v>
@@ -3083,27 +3101,27 @@
         <v>21</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>12</v>
@@ -3112,7 +3130,7 @@
         <v>19</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="J40" s="12" t="s">
         <v>21</v>
@@ -3121,27 +3139,27 @@
         <v>21</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>228</v>
+        <v>49</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>12</v>
@@ -3150,7 +3168,7 @@
         <v>19</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>21</v>
@@ -3159,27 +3177,27 @@
         <v>21</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>12</v>
@@ -3188,7 +3206,7 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="J42" s="12" t="s">
         <v>21</v>
@@ -3197,27 +3215,27 @@
         <v>21</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>12</v>
@@ -3226,7 +3244,7 @@
         <v>19</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>21</v>
@@ -3235,18 +3253,18 @@
         <v>21</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>234</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>241</v>
@@ -3255,7 +3273,7 @@
         <v>242</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>12</v>
@@ -3264,7 +3282,7 @@
         <v>19</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>21</v>
@@ -3273,27 +3291,27 @@
         <v>21</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>247</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>12</v>
@@ -3302,7 +3320,7 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="J45" s="8" t="s">
         <v>21</v>
@@ -3311,15 +3329,15 @@
         <v>21</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>250</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>251</v>
@@ -3350,6 +3368,44 @@
       </c>
       <c r="L46" s="10" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30" customHeight="1">
+      <c r="A47" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -3364,7 +3420,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -3386,7 +3442,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3394,13 +3450,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3408,13 +3464,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3423,38 +3479,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G47)</f>
+        <f>SUM(G10:G48)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3474,16 +3530,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3791,7 +3847,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1">
+    <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
         <v>121</v>
       </c>
@@ -3801,34 +3857,31 @@
       <c r="C24" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>124</v>
-      </c>
       <c r="E24" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
       </c>
       <c r="G24" s="20">
         <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="30" customHeight="1">
       <c r="A25" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>132</v>
-      </c>
       <c r="E25" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G25" s="20">
         <f>IF(AND(ISNUMBER(E25),ISNUMBER(F25)),E25*F25,"")</f>
@@ -3837,16 +3890,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>138</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>140</v>
       </c>
       <c r="E26" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3857,22 +3910,22 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="D27" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>148</v>
-      </c>
       <c r="E27" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G27" s="20">
         <f>IF(AND(ISNUMBER(E27),ISNUMBER(F27)),E27*F27,"")</f>
@@ -3881,16 +3934,16 @@
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="D28" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>156</v>
       </c>
       <c r="E28" s="19">
         <f>BoardQty*1</f>
@@ -3901,7 +3954,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" ht="30" customHeight="1">
       <c r="A29" s="19" t="s">
         <v>159</v>
       </c>
@@ -3923,18 +3976,18 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>166</v>
       </c>
       <c r="C30" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>168</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>169</v>
       </c>
       <c r="E30" s="19">
         <f>BoardQty*1</f>
@@ -3947,16 +4000,16 @@
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
       <c r="A31" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>175</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>177</v>
       </c>
       <c r="E31" s="19">
         <f>BoardQty*1</f>
@@ -3969,32 +4022,32 @@
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
       <c r="A32" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>185</v>
-      </c>
       <c r="E32" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G32" s="20">
         <f>IF(AND(ISNUMBER(E32),ISNUMBER(F32)),E32*F32,"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" ht="30" customHeight="1">
       <c r="A33" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>189</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>188</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>190</v>
@@ -4003,8 +4056,8 @@
         <v>191</v>
       </c>
       <c r="E33" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G33" s="20">
         <f>IF(AND(ISNUMBER(E33),ISNUMBER(F33)),E33*F33,"")</f>
@@ -4013,16 +4066,16 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>198</v>
       </c>
       <c r="E34" s="19">
         <f>BoardQty*1</f>
@@ -4035,16 +4088,16 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>202</v>
+        <v>72</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E35" s="19">
         <f>BoardQty*1</f>
@@ -4057,16 +4110,16 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="19" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E36" s="19">
         <f>BoardQty*1</f>
@@ -4079,27 +4132,27 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E37" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G37" s="20">
         <f>IF(AND(ISNUMBER(E37),ISNUMBER(F37)),E37*F37,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="30" customHeight="1">
+    <row r="38" spans="1:7">
       <c r="A38" s="19" t="s">
         <v>215</v>
       </c>
@@ -4107,14 +4160,14 @@
         <v>216</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="E38" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G38" s="20">
         <f>IF(AND(ISNUMBER(E38),ISNUMBER(F38)),E38*F38,"")</f>
@@ -4129,10 +4182,10 @@
         <v>222</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E39" s="19">
         <f>BoardQty*1</f>
@@ -4145,16 +4198,16 @@
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
       <c r="A40" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>224</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>218</v>
       </c>
       <c r="E40" s="19">
         <f>BoardQty*1</f>
@@ -4167,16 +4220,16 @@
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
       <c r="A41" s="19" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E41" s="19">
         <f>BoardQty*1</f>
@@ -4189,16 +4242,16 @@
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>228</v>
+        <v>49</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E42" s="19">
         <f>BoardQty*1</f>
@@ -4211,16 +4264,16 @@
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E43" s="19">
         <f>BoardQty*1</f>
@@ -4233,16 +4286,16 @@
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="E44" s="19">
         <f>BoardQty*1</f>
@@ -4261,10 +4314,10 @@
         <v>242</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="E45" s="19">
         <f>BoardQty*1</f>
@@ -4277,16 +4330,16 @@
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
       <c r="A46" s="19" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E46" s="19">
         <f>BoardQty*1</f>
@@ -4319,17 +4372,39 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>282</v>
+    <row r="48" spans="1:7" ht="30" customHeight="1">
+      <c r="A48" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="E48" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G48" s="20">
+        <f>IF(AND(ISNUMBER(E48),ISNUMBER(F48)),E48*F48,"")</f>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="23" t="s">
-        <v>283</v>
+      <c r="A51" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="23" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -4527,6 +4602,11 @@
       <formula>AND(ISBLANK(D47),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="expression" dxfId="0" priority="39">
+      <formula>AND(ISBLANK(D48),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -4541,30 +4621,30 @@
     <hyperlink ref="D21" r:id="rId11"/>
     <hyperlink ref="D22" r:id="rId12"/>
     <hyperlink ref="D23" r:id="rId13"/>
-    <hyperlink ref="D24" r:id="rId14"/>
-    <hyperlink ref="D25" r:id="rId15"/>
-    <hyperlink ref="D26" r:id="rId16"/>
-    <hyperlink ref="D27" r:id="rId17"/>
-    <hyperlink ref="D28" r:id="rId18"/>
-    <hyperlink ref="D29" r:id="rId19"/>
-    <hyperlink ref="D30" r:id="rId20"/>
-    <hyperlink ref="D31" r:id="rId21"/>
-    <hyperlink ref="D32" r:id="rId22"/>
-    <hyperlink ref="D33" r:id="rId23"/>
-    <hyperlink ref="D34" r:id="rId24"/>
-    <hyperlink ref="D35" r:id="rId25"/>
-    <hyperlink ref="D36" r:id="rId26"/>
-    <hyperlink ref="D37" r:id="rId27"/>
-    <hyperlink ref="D38" r:id="rId28"/>
-    <hyperlink ref="D39" r:id="rId29"/>
-    <hyperlink ref="D40" r:id="rId30"/>
-    <hyperlink ref="D41" r:id="rId31"/>
-    <hyperlink ref="D42" r:id="rId32"/>
-    <hyperlink ref="D43" r:id="rId33"/>
-    <hyperlink ref="D44" r:id="rId34"/>
-    <hyperlink ref="D45" r:id="rId35"/>
-    <hyperlink ref="D46" r:id="rId36"/>
-    <hyperlink ref="D47" r:id="rId37"/>
+    <hyperlink ref="D25" r:id="rId14"/>
+    <hyperlink ref="D26" r:id="rId15"/>
+    <hyperlink ref="D27" r:id="rId16"/>
+    <hyperlink ref="D28" r:id="rId17"/>
+    <hyperlink ref="D29" r:id="rId18"/>
+    <hyperlink ref="D30" r:id="rId19"/>
+    <hyperlink ref="D31" r:id="rId20"/>
+    <hyperlink ref="D32" r:id="rId21"/>
+    <hyperlink ref="D33" r:id="rId22"/>
+    <hyperlink ref="D34" r:id="rId23"/>
+    <hyperlink ref="D35" r:id="rId24"/>
+    <hyperlink ref="D36" r:id="rId25"/>
+    <hyperlink ref="D37" r:id="rId26"/>
+    <hyperlink ref="D38" r:id="rId27"/>
+    <hyperlink ref="D39" r:id="rId28"/>
+    <hyperlink ref="D40" r:id="rId29"/>
+    <hyperlink ref="D41" r:id="rId30"/>
+    <hyperlink ref="D42" r:id="rId31"/>
+    <hyperlink ref="D43" r:id="rId32"/>
+    <hyperlink ref="D44" r:id="rId33"/>
+    <hyperlink ref="D45" r:id="rId34"/>
+    <hyperlink ref="D46" r:id="rId35"/>
+    <hyperlink ref="D47" r:id="rId36"/>
+    <hyperlink ref="D48" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId38"/>
@@ -4585,72 +4665,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@e5364ac2dec5f234752869372469cf630962c8e1 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -8,13 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
-    <sheet name="Costs" sheetId="2" r:id="rId2"/>
-    <sheet name="Colors" sheetId="3" r:id="rId3"/>
+    <sheet name="DNF" sheetId="2" r:id="rId2"/>
+    <sheet name="Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="Costs (DNF)" sheetId="4" r:id="rId4"/>
+    <sheet name="Colors" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="1">'Costs'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="2">'Costs'!$G$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="1">'Costs'!$G$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
+    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="2">'Costs'!$G$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -139,8 +144,127 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use the minimum extend price across distributors not taking account available quantities.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schematic identifier for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PCB footprint for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manufacturer number for each part and link to it's datasheet (Ctrl-click).
+Purple -&gt; Obsolete part detected by one of the distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of each part needed.
+Gray -&gt; No manf# provided.
+Red -&gt; No parts available.
+Orange -&gt; Not enough parts available.
+Yellow -&gt; Parts available, but haven't purchased enough.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum unit price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum extended price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="307">
   <si>
     <t>Row</t>
   </si>
@@ -349,7 +473,7 @@
     <t>NeoPixel_THT</t>
   </si>
   <si>
-    <t>D1 D2 D3 D4 D5 D6 D7 D8 D9 D10</t>
+    <t>D1 D2 D3 D4</t>
   </si>
   <si>
     <t>NEOPIX</t>
@@ -358,39 +482,39 @@
     <t>LED_D5.0mm-NeoPixel</t>
   </si>
   <si>
+    <t>https://cdn.sparkfun.com/assets/6/9/0/f/3/DS-12999-LED_-_RGB_Addressable__PTH__5mm_Clear__5_Pack_.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/sparkfun-electronics/COM-12999/5673800</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Resettable fuse, polymeric positive temperature coefficient</t>
+  </si>
+  <si>
+    <t>Polyfuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Polyfuse 1.8A</t>
+  </si>
+  <si>
+    <t>C_Rect_L7.0mm_W3.5mm_P5.00mm</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/1n5400-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bel-fuse-inc/0ZRP0090FF1E/9468255</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
-    <t>https://cdn.sparkfun.com/assets/6/9/0/f/3/DS-12999-LED_-_RGB_Addressable__PTH__5mm_Clear__5_Pack_.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/sparkfun-electronics/COM-12999/5673800</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Resettable fuse, polymeric positive temperature coefficient</t>
-  </si>
-  <si>
-    <t>Polyfuse</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Polyfuse 1.8A</t>
-  </si>
-  <si>
-    <t>C_Rect_L7.0mm_W3.5mm_P5.00mm</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/1n5400-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/bel-fuse-inc/0ZRP0090FF1E/9468255</t>
-  </si>
-  <si>
     <t>Fuse, small symbol</t>
   </si>
   <si>
@@ -511,7 +635,7 @@
     <t>LED-Ring</t>
   </si>
   <si>
-    <t>PinHeader_2x02_P2.00mm_Vertical</t>
+    <t>Led-Ring</t>
   </si>
   <si>
     <t>16</t>
@@ -973,12 +1097,21 @@
     <t>Fitted Components:</t>
   </si>
   <si>
+    <t>76 (4 SMD/ 70 THT)</t>
+  </si>
+  <si>
     <t>Number of PCBs:</t>
   </si>
   <si>
     <t>Total Components:</t>
   </si>
   <si>
+    <t>D5 D6 D7 D8 D9 D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -1006,7 +1139,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-09 15:09:11</t>
+    <t>2023-06-12 14:27:04</t>
   </si>
   <si>
     <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
@@ -1454,8 +1587,112 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1464384</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2378784</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>454734</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1829,7 +2066,7 @@
         <v>273</v>
       </c>
       <c r="F2" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1857,7 +2094,7 @@
         <v>276</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1868,7 +2105,7 @@
         <v>270</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1882,10 +2119,10 @@
         <v>272</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F6" s="3">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2212,42 +2449,42 @@
         <v>71</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>12</v>
@@ -2256,21 +2493,21 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="9" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>83</v>
@@ -2890,7 +3127,7 @@
         <v>202</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>203</v>
@@ -3419,6 +3656,201 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="60.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="32" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="C2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="C3" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="C4" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="C5" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="C6" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F6" s="3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G52"/>
   <sheetViews>
@@ -3456,7 +3888,7 @@
         <v>264</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3470,7 +3902,7 @@
         <v>266</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3485,7 +3917,7 @@
         <v>268</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G48)</f>
@@ -3510,7 +3942,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3530,16 +3962,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -3707,11 +4139,11 @@
         <v>71</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="19">
-        <f>CEILING(BoardQty*10,1)</f>
-        <v>10</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G17" s="20">
         <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
@@ -3720,16 +4152,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>80</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>81</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -4091,7 +4523,7 @@
         <v>202</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>203</v>
@@ -4396,15 +4828,15 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="21" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="23" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -4652,7 +5084,184 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="57.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="32" customHeight="1">
+      <c r="D1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="D2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="G3" s="15">
+        <f>TotalCost/BoardQty</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="G4" s="16">
+        <f>SUM(G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1">
+      <c r="A10" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="19">
+        <f>CEILING(BoardQty*6,1)</f>
+        <v>6</v>
+      </c>
+      <c r="G10" s="20">
+        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(ISBLANK(D10),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -4665,72 +5274,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@9fa64109e6f198db5dd7bff9b4a6257a63a77d4c 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1139,10 +1139,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-06-12 15:25:55</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.17 + KiBot v1.6.2</t>
+    <t>2023-07-09 16:37:20</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@d2d4a34964746bc5a78dd8214c9f7561b88935d0 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1082,7 +1082,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.5.1-1-g8f565ef7f0-dirty-deb11</t>
+    <t>7.0.7-7.0.7~ubuntu23.04.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -1139,7 +1139,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-07-18 10:36:12</t>
+    <t>2023-09-09 12:20:14</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -3669,7 +3669,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -3865,9 +3865,9 @@
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="3" max="3" width="54.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
@@ -5100,7 +5100,7 @@
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="57.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="34.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@07bb7b7d0296cf0ecf3347f2f5c02306554c12c2 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1152,13 +1152,13 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>2.1.0-RC1</t>
+    <t>2.1.0</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-03-12</t>
+    <t>2023-09-10</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -1224,7 +1224,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-09-10 09:48:11</t>
+    <t>2023-09-10 10:07:25</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@c72273cca7806562fde3afadfa035133cc8ede57 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/pedalboard-hw-bom.xlsx
+++ b/BoM/Costs/pedalboard-hw-bom.xlsx
@@ -1152,7 +1152,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>2.1.0</t>
+    <t>3.0.0-RC1</t>
   </si>
   <si>
     <t>Date:</t>
@@ -1224,7 +1224,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-09-10 11:40:44</t>
+    <t>2023-09-10 11:54:45</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>